<commit_message>
changing logic, resetting index
</commit_message>
<xml_diff>
--- a/general_data/mgc_plant_clusters.xlsx
+++ b/general_data/mgc_plant_clusters.xlsx
@@ -496,7 +496,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>BGC0002394</t>
+          <t>BGC0000669</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -511,14 +511,14 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Taxus chinensis</t>
+          <t>Arabidopsis thaliana</t>
         </is>
       </c>
       <c r="F2" t="n">
-        <v>55305454</v>
+        <v>17023645</v>
       </c>
       <c r="G2" t="n">
-        <v>55566904</v>
+        <v>17058245</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
@@ -526,7 +526,7 @@
         </is>
       </c>
       <c r="I2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -535,22 +535,22 @@
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Taxus chinensis isolate Ta-2019 chromosome 9, whole genome shotgun sequence</t>
+          <t>Arabidopsis thaliana chromosome 5 sequence</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>taxa-4(20),11(12)-diene,</t>
+          <t>marneral</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>BGC0000810</t>
+          <t>BGC0000670</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -565,14 +565,14 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Zea mays</t>
+          <t>Arabidopsis thaliana</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>3003161</v>
+        <v>19428887</v>
       </c>
       <c r="G3" t="n">
-        <v>3267368</v>
+        <v>19461689</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -580,31 +580,31 @@
         </is>
       </c>
       <c r="I3" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Alkaloid</t>
+          <t>Terpene</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Zea mays cultivar B73 chromosome 4</t>
+          <t>Arabidopsis thaliana chromosome 5 sequence</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>benzoxazinone</t>
+          <t>thaliandiol,</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>BGC0002395</t>
+          <t>BGC0000671</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -619,14 +619,14 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Hordeum vulgare subsp. vulgare</t>
+          <t>Oryza sativa Japonica Group</t>
         </is>
       </c>
       <c r="F4" t="n">
-        <v>9581241</v>
+        <v>5310456</v>
       </c>
       <c r="G4" t="n">
-        <v>10180879</v>
+        <v>5479082</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -634,7 +634,7 @@
         </is>
       </c>
       <c r="I4" t="n">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -643,22 +643,22 @@
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Hordeum vulgare subsp. vulgare chromosome 2H, MorexV3_pseudomolecules_assembly, whole genome shotgun sequence</t>
+          <t>Oryza sativa Japonica Group DNA, chromosome 4, complete sequence, cultivar: Nipponbare</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>11-hydroxy-hordetriene,</t>
+          <t>momilactone</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>BGC0001313</t>
+          <t>BGC0000672</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -673,14 +673,14 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana</t>
+          <t>Oryza sativa Japonica Group</t>
         </is>
       </c>
       <c r="F5" t="n">
-        <v>8729999</v>
+        <v>22520468</v>
       </c>
       <c r="G5" t="n">
-        <v>8820000</v>
+        <v>22764099</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -688,7 +688,7 @@
         </is>
       </c>
       <c r="I5" t="n">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -697,22 +697,22 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana chromosome 4 sequence</t>
+          <t>Oryza sativa Japonica Group DNA, chromosome 2, complete sequence, cultivar: Nipponbare</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>arabidiol-baruol</t>
+          <t>oryzalides,</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BGC0002622</t>
+          <t>BGC0000810</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -727,14 +727,14 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Oryza sativa Japonica Group</t>
+          <t>Zea mays</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>21409012</v>
+        <v>3003161</v>
       </c>
       <c r="G6" t="n">
-        <v>21465464</v>
+        <v>3267368</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -742,31 +742,31 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Alkaloid</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Oryza sativa Japonica Group DNA, chromosome 9, cultivar: Nipponbare, complete sequence</t>
+          <t>Zea mays cultivar B73 chromosome 4</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>hydroxycinnamoylputrescine</t>
+          <t>benzoxazinone</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BGC0001317</t>
+          <t>BGC0001313</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -781,14 +781,14 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Lotus japonicus</t>
+          <t>Arabidopsis thaliana</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>0</v>
+        <v>8729999</v>
       </c>
       <c r="G7" t="n">
-        <v>277585</v>
+        <v>8820000</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -805,22 +805,22 @@
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Lupeol biosynthetic gene cluster</t>
+          <t>Arabidopsis thaliana chromosome 4 sequence</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>lupeol</t>
+          <t>arabidiol-baruol</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BGC0002391</t>
+          <t>BGC0001314</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -835,14 +835,14 @@
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Zea mays</t>
+          <t>Arabidopsis thaliana</t>
         </is>
       </c>
       <c r="F8" t="n">
-        <v>285583113</v>
+        <v>14189999</v>
       </c>
       <c r="G8" t="n">
-        <v>285654925</v>
+        <v>14250000</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -850,7 +850,7 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -859,44 +859,44 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Zea mays cultivar B73 chromosome 1, Zm-B73-REFERENCE-NAM-5.0, whole genome shotgun sequence</t>
+          <t>Arabidopsis thaliana chromosome 5 sequence</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>zealexin</t>
+          <t>tirucalla</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>BGC0001315</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>Cucumis sativus</t>
+        </is>
+      </c>
+      <c r="F9" t="n">
         <v>0</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>BGC0002390</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Zea mays</t>
-        </is>
-      </c>
-      <c r="F9" t="n">
-        <v>33367131</v>
-      </c>
       <c r="G9" t="n">
-        <v>34010443</v>
+        <v>35297</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -904,7 +904,7 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -913,18 +913,18 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Zea mays cultivar B73 chromosome 5, Zm-B73-REFERENCE-NAM-5.0, whole genome shotgun sequence</t>
+          <t>Cucurbitacin biosynthetic gene cluster</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>zealexin</t>
+          <t>cucurbitacin</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
@@ -978,33 +978,33 @@
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>BGC0001317</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Lotus japonicus</t>
+        </is>
+      </c>
+      <c r="F11" t="n">
         <v>0</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>BGC0001314</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Arabidopsis thaliana</t>
-        </is>
-      </c>
-      <c r="F11" t="n">
-        <v>14189999</v>
-      </c>
       <c r="G11" t="n">
-        <v>14250000</v>
+        <v>277585</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -1012,7 +1012,7 @@
         </is>
       </c>
       <c r="I11" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -1021,44 +1021,44 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana chromosome 5 sequence</t>
+          <t>Lupeol biosynthetic gene cluster</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>tirucalla</t>
+          <t>lupeol</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>BGC0001318</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Manihot esculenta</t>
+        </is>
+      </c>
+      <c r="F12" t="n">
         <v>0</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>BGC0002392</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Oryza sativa Japonica Group</t>
-        </is>
-      </c>
-      <c r="F12" t="n">
-        <v>6494479</v>
-      </c>
       <c r="G12" t="n">
-        <v>6634480</v>
+        <v>80994</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -1066,53 +1066,53 @@
         </is>
       </c>
       <c r="I12" t="n">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Oryza sativa Japonica Group DNA, chromosome 7, cultivar: Nipponbare, complete sequence</t>
+          <t>Linamarin / Lotaustralin biosynthetic gene cluster</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>5,10-diketo-casbene</t>
+          <t>linamarin,</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>BGC0001324</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>Solanum pimpinellifolium</t>
+        </is>
+      </c>
+      <c r="F13" t="n">
         <v>0</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>BGC0002393</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Ricinus communis</t>
-        </is>
-      </c>
-      <c r="F13" t="n">
-        <v>264511</v>
-      </c>
       <c r="G13" t="n">
-        <v>337591</v>
+        <v>107124</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -1120,7 +1120,7 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>17</v>
+        <v>0</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1129,22 +1129,22 @@
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Ricinus communis genomic scaffold scf_1106159296192, whole genome shotgun sequence</t>
+          <t>Solanum pimpinellifolium isolate LA1589 chromosome 8 terpene biosynthesis gene locus, partial sequence</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>5a-hydroxy-casbene,</t>
+          <t>monoterpenes-diterpenes</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>BGC0001315</t>
+          <t>BGC0001325</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1159,14 +1159,14 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Cucumis sativus</t>
+          <t>Papaver somniferum</t>
         </is>
       </c>
       <c r="F14" t="n">
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>35297</v>
+        <v>401328</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -1174,31 +1174,31 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>Alkaloid</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Cucurbitacin biosynthetic gene cluster</t>
+          <t>Noscapine biosynthetic gene cluster</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>cucurbitacin</t>
+          <t>noscapine</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BGC0000669</t>
+          <t>BGC0001756</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1217,10 +1217,10 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>17023645</v>
+        <v>4863612</v>
       </c>
       <c r="G15" t="n">
-        <v>17058245</v>
+        <v>4887487</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -1228,7 +1228,7 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1237,22 +1237,22 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana chromosome 5 sequence</t>
+          <t>Arabidopsis thaliana chromosome 3, partial sequence</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>marneral</t>
+          <t>arathanatriene,</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BGC0002724</t>
+          <t>BGC0001799</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1267,14 +1267,14 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Jatropha curcas</t>
+          <t>Papaver somniferum</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>848628</v>
+        <v>78651</v>
       </c>
       <c r="G16" t="n">
-        <v>912207</v>
+        <v>1013747</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1282,85 +1282,85 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>Alkaloid</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Jatropha curcas isolate ELGS0001-1231 unplaced genomic scaffold, RJC1_Hi-C scaffold_989, whole genome shotgun sequence</t>
+          <t>UNVERIFIED: Papaver somniferum (S)-reticuline epimerase-like (REPI1), REPI2, salutaridine synthase (SalSyn1), O-methyltransferase-1, SalSyn2, O-methyltransferase-2, salutaridinol 7-O-acetyltransferase (SalAT2), salutaridine reductase-like (SalR2), and thebaine synthase 2 (THS2) genes, partial sequence; thebaine synthase 1-like (THS1) gene, complete sequence; and SalR1 and SalAT1 genes, partial sequence</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>casbene</t>
+          <t>thebaine</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>BGC0001997</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Nicotiana tabacum</t>
+        </is>
+      </c>
+      <c r="F17" t="n">
+        <v>469295</v>
+      </c>
+      <c r="G17" t="n">
+        <v>543944</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I17" t="n">
         <v>0</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>BGC0002721</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Hordeum vulgare subsp. vulgare</t>
-        </is>
-      </c>
-      <c r="F17" t="n">
-        <v>17320184</v>
-      </c>
-      <c r="G17" t="n">
-        <v>17862889</v>
-      </c>
-      <c r="H17" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I17" t="n">
-        <v>5</v>
-      </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Saccharide</t>
+          <t>Terpene</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Hordeum vulgare subsp. vulgare chromosome 1H, MorexV3_pseudomolecules_assembly, whole genome shotgun sequence</t>
+          <t>Nicotiana tabacum cultivar K326 Nitab4.5_0001461, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>α-hydroxynitrile</t>
+          <t>capsidiol</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BGC0001997</t>
+          <t>BGC0002389</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1375,14 +1375,14 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Nicotiana tabacum</t>
+          <t>Zea mays</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>469295</v>
+        <v>56565232</v>
       </c>
       <c r="G18" t="n">
-        <v>543944</v>
+        <v>56847613</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1390,7 +1390,7 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1399,22 +1399,22 @@
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Nicotiana tabacum cultivar K326 Nitab4.5_0001461, whole genome shotgun sequence</t>
+          <t>Zea mays cultivar B73 chromosome 10, Zm-B73-REFERENCE-NAM-5.0, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>capsidiol</t>
+          <t>β-bisabolene,</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BGC0002722</t>
+          <t>BGC0002390</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1429,14 +1429,14 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Saccharide</t>
+          <t>Zea mays</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>1123004</v>
+        <v>33367131</v>
       </c>
       <c r="G19" t="n">
-        <v>1460949</v>
+        <v>34010443</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1444,31 +1444,31 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Alkaloid</t>
+          <t>Terpene</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Solanum tuberosum cultivar DM 1-3 516 R44 unplaced genomic scaffold, SolTub_3.0 scf00140, whole genome shotgun sequence</t>
+          <t>Zea mays cultivar B73 chromosome 5, Zm-B73-REFERENCE-NAM-5.0, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>α-chaconine,</t>
+          <t>zealexin</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BGC0002723</t>
+          <t>BGC0002391</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1483,14 +1483,14 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Jatropha curcas</t>
+          <t>Zea mays</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>7856</v>
+        <v>285583113</v>
       </c>
       <c r="G20" t="n">
-        <v>18675</v>
+        <v>285654925</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1507,22 +1507,22 @@
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Jatropha curcas isolate ELGS0001-1231 unplaced genomic scaffold, RJC1_Hi-C scaffold_928, whole genome shotgun sequence</t>
+          <t>Zea mays cultivar B73 chromosome 1, Zm-B73-REFERENCE-NAM-5.0, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>casbene</t>
+          <t>zealexin</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BGC0001799</t>
+          <t>BGC0002392</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1537,14 +1537,14 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Papaver somniferum</t>
+          <t>Oryza sativa Japonica Group</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>78651</v>
+        <v>6494479</v>
       </c>
       <c r="G21" t="n">
-        <v>1013747</v>
+        <v>6634480</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1552,31 +1552,31 @@
         </is>
       </c>
       <c r="I21" t="n">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Alkaloid</t>
+          <t>Terpene</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>UNVERIFIED: Papaver somniferum (S)-reticuline epimerase-like (REPI1), REPI2, salutaridine synthase (SalSyn1), O-methyltransferase-1, SalSyn2, O-methyltransferase-2, salutaridinol 7-O-acetyltransferase (SalAT2), salutaridine reductase-like (SalR2), and thebaine synthase 2 (THS2) genes, partial sequence; thebaine synthase 1-like (THS1) gene, complete sequence; and SalR1 and SalAT1 genes, partial sequence</t>
+          <t>Oryza sativa Japonica Group DNA, chromosome 7, cultivar: Nipponbare, complete sequence</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>thebaine</t>
+          <t>5,10-diketo-casbene</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BGC0001756</t>
+          <t>BGC0002393</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1591,14 +1591,14 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana</t>
+          <t>Ricinus communis</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>4863612</v>
+        <v>264511</v>
       </c>
       <c r="G22" t="n">
-        <v>4887487</v>
+        <v>337591</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
@@ -1606,7 +1606,7 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1615,22 +1615,22 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana chromosome 3, partial sequence</t>
+          <t>Ricinus communis genomic scaffold scf_1106159296192, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>arathanatriene,</t>
+          <t>5a-hydroxy-casbene,</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BGC0000671</t>
+          <t>BGC0002394</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1645,14 +1645,14 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Oryza sativa Japonica Group</t>
+          <t>Taxus chinensis</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>5310456</v>
+        <v>55305454</v>
       </c>
       <c r="G23" t="n">
-        <v>5479082</v>
+        <v>55566904</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -1660,7 +1660,7 @@
         </is>
       </c>
       <c r="I23" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1669,22 +1669,22 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Oryza sativa Japonica Group DNA, chromosome 4, complete sequence, cultivar: Nipponbare</t>
+          <t>Taxus chinensis isolate Ta-2019 chromosome 9, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>momilactone</t>
+          <t>taxa-4(20),11(12)-diene,</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BGC0000670</t>
+          <t>BGC0002395</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1699,14 +1699,14 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana</t>
+          <t>Hordeum vulgare subsp. vulgare</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>19428887</v>
+        <v>9581241</v>
       </c>
       <c r="G24" t="n">
-        <v>19461689</v>
+        <v>10180879</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -1714,7 +1714,7 @@
         </is>
       </c>
       <c r="I24" t="n">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1723,22 +1723,22 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana chromosome 5 sequence</t>
+          <t>Hordeum vulgare subsp. vulgare chromosome 2H, MorexV3_pseudomolecules_assembly, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>thaliandiol,</t>
+          <t>11-hydroxy-hordetriene,</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>BGC0000672</t>
+          <t>BGC0002404</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1753,14 +1753,14 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Oryza sativa Japonica Group</t>
+          <t>Solanum lycopersicum</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>22520468</v>
+        <v>68007492</v>
       </c>
       <c r="G25" t="n">
-        <v>22764099</v>
+        <v>68031028</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
@@ -1768,31 +1768,31 @@
         </is>
       </c>
       <c r="I25" t="n">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Oryza sativa Japonica Group DNA, chromosome 2, complete sequence, cultivar: Nipponbare</t>
+          <t>Solanum lycopersicum cultivar Heinz 1706 chromosome 12, SL3.0, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>oryzalides,</t>
+          <t>falcarindiol</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BGC0001324</t>
+          <t>BGC0002405</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1807,14 +1807,14 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Solanum pimpinellifolium</t>
+          <t>Solanum lycopersicum</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>0</v>
+        <v>57739269</v>
       </c>
       <c r="G26" t="n">
-        <v>107124</v>
+        <v>57782130</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
@@ -1822,31 +1822,31 @@
         </is>
       </c>
       <c r="I26" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>Saccharide</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Solanum pimpinellifolium isolate LA1589 chromosome 8 terpene biosynthesis gene locus, partial sequence</t>
+          <t>Solanum lycopersicum cultivar Heinz 1706 chromosome 7, SL3.0, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>monoterpenes-diterpenes</t>
+          <t>mid-chain</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>BGC0001318</t>
+          <t>BGC0002406</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1861,14 +1861,14 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Manihot esculenta</t>
+          <t>Oryza sativa Japonica Group</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>0</v>
+        <v>12067615</v>
       </c>
       <c r="G27" t="n">
-        <v>80994</v>
+        <v>12262361</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -1876,7 +1876,7 @@
         </is>
       </c>
       <c r="I27" t="n">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -1885,22 +1885,22 @@
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Linamarin / Lotaustralin biosynthetic gene cluster</t>
+          <t>Oryza sativa Japonica Group DNA, chromosome 10, cultivar: Nipponbare, complete sequence</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>linamarin,</t>
+          <t>hydroxycinnamoyltyramine</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>0</v>
+        <v>26</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>BGC0002406</t>
+          <t>BGC0002622</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1919,10 +1919,10 @@
         </is>
       </c>
       <c r="F28" t="n">
-        <v>12067615</v>
+        <v>21409012</v>
       </c>
       <c r="G28" t="n">
-        <v>12262361</v>
+        <v>21465464</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
@@ -1930,7 +1930,7 @@
         </is>
       </c>
       <c r="I28" t="n">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -1939,22 +1939,22 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Oryza sativa Japonica Group DNA, chromosome 10, cultivar: Nipponbare, complete sequence</t>
+          <t>Oryza sativa Japonica Group DNA, chromosome 9, cultivar: Nipponbare, complete sequence</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>hydroxycinnamoyltyramine</t>
+          <t>hydroxycinnamoylputrescine</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>BGC0001325</t>
+          <t>BGC0002721</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1969,14 +1969,14 @@
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Papaver somniferum</t>
+          <t>Hordeum vulgare subsp. vulgare</t>
         </is>
       </c>
       <c r="F29" t="n">
-        <v>0</v>
+        <v>17320184</v>
       </c>
       <c r="G29" t="n">
-        <v>401328</v>
+        <v>17862889</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
@@ -1984,31 +1984,31 @@
         </is>
       </c>
       <c r="I29" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Alkaloid</t>
+          <t>Saccharide</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Noscapine biosynthetic gene cluster</t>
+          <t>Hordeum vulgare subsp. vulgare chromosome 1H, MorexV3_pseudomolecules_assembly, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>noscapine</t>
+          <t>α-hydroxynitrile</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>0</v>
+        <v>28</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BGC0002389</t>
+          <t>BGC0002722</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2023,14 +2023,14 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Zea mays</t>
+          <t>Saccharide</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>56565232</v>
+        <v>1123004</v>
       </c>
       <c r="G30" t="n">
-        <v>56847613</v>
+        <v>1460949</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
@@ -2038,31 +2038,31 @@
         </is>
       </c>
       <c r="I30" t="n">
-        <v>4</v>
+        <v>22</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>Alkaloid</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Zea mays cultivar B73 chromosome 10, Zm-B73-REFERENCE-NAM-5.0, whole genome shotgun sequence</t>
+          <t>Solanum tuberosum cultivar DM 1-3 516 R44 unplaced genomic scaffold, SolTub_3.0 scf00140, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>β-bisabolene,</t>
+          <t>α-chaconine,</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>BGC0002404</t>
+          <t>BGC0002723</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2077,14 +2077,14 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Solanum lycopersicum</t>
+          <t>Jatropha curcas</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>68007492</v>
+        <v>7856</v>
       </c>
       <c r="G31" t="n">
-        <v>68031028</v>
+        <v>18675</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
@@ -2092,31 +2092,31 @@
         </is>
       </c>
       <c r="I31" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Terpene</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Solanum lycopersicum cultivar Heinz 1706 chromosome 12, SL3.0, whole genome shotgun sequence</t>
+          <t>Jatropha curcas isolate ELGS0001-1231 unplaced genomic scaffold, RJC1_Hi-C scaffold_928, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>falcarindiol</t>
+          <t>casbene</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>BGC0002405</t>
+          <t>BGC0002724</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
@@ -2131,14 +2131,14 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>Solanum lycopersicum</t>
+          <t>Jatropha curcas</t>
         </is>
       </c>
       <c r="F32" t="n">
-        <v>57739269</v>
+        <v>848628</v>
       </c>
       <c r="G32" t="n">
-        <v>57782130</v>
+        <v>912207</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
@@ -2146,21 +2146,21 @@
         </is>
       </c>
       <c r="I32" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Saccharide</t>
+          <t>Terpene</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Solanum lycopersicum cultivar Heinz 1706 chromosome 7, SL3.0, whole genome shotgun sequence</t>
+          <t>Jatropha curcas isolate ELGS0001-1231 unplaced genomic scaffold, RJC1_Hi-C scaffold_989, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>mid-chain</t>
+          <t>casbene</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
adding json logic, still need to implement json
</commit_message>
<xml_diff>
--- a/general_data/mgc_plant_clusters.xlsx
+++ b/general_data/mgc_plant_clusters.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:M45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,6 +489,11 @@
           <t>main_product</t>
         </is>
       </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>mibig_version</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -543,6 +548,11 @@
           <t>marneral</t>
         </is>
       </c>
+      <c r="M2" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -597,6 +607,11 @@
           <t>thaliandiol,</t>
         </is>
       </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -651,6 +666,11 @@
           <t>momilactone</t>
         </is>
       </c>
+      <c r="M4" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -705,6 +725,11 @@
           <t>oryzalides,</t>
         </is>
       </c>
+      <c r="M5" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -712,7 +737,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>BGC0000810</t>
+          <t>BGC0000798</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -727,14 +752,14 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Zea mays</t>
+          <t>Sorghum bicolor</t>
         </is>
       </c>
       <c r="F6" t="n">
-        <v>3003161</v>
+        <v>1058884</v>
       </c>
       <c r="G6" t="n">
-        <v>3267368</v>
+        <v>1163330</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
@@ -742,21 +767,26 @@
         </is>
       </c>
       <c r="I6" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Alkaloid</t>
+          <t>Saccharide</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Zea mays cultivar B73 chromosome 4</t>
+          <t>Sorghum bicolor chromosome 1, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>benzoxazinone</t>
+          <t>dhurrin</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.0</t>
         </is>
       </c>
     </row>
@@ -766,7 +796,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>BGC0001313</t>
+          <t>BGC0000810</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -781,14 +811,14 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana</t>
+          <t>Zea mays</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>8729999</v>
+        <v>3003161</v>
       </c>
       <c r="G7" t="n">
-        <v>8820000</v>
+        <v>3267368</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -796,21 +826,26 @@
         </is>
       </c>
       <c r="I7" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>Alkaloid</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana chromosome 4 sequence</t>
+          <t>Zea mays cultivar B73 chromosome 4</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>arabidiol-baruol</t>
+          <t>benzoxazinone</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>
@@ -820,7 +855,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>BGC0001314</t>
+          <t>BGC0001313</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -839,10 +874,10 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>14189999</v>
+        <v>8729999</v>
       </c>
       <c r="G8" t="n">
-        <v>14250000</v>
+        <v>8820000</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
@@ -850,7 +885,7 @@
         </is>
       </c>
       <c r="I8" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -859,12 +894,17 @@
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana chromosome 5 sequence</t>
+          <t>Arabidopsis thaliana chromosome 4 sequence</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>tirucalla</t>
+          <t>arabidiol-baruol</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>
@@ -874,7 +914,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>BGC0001315</t>
+          <t>BGC0001314</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -889,14 +929,14 @@
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Cucumis sativus</t>
+          <t>Arabidopsis thaliana</t>
         </is>
       </c>
       <c r="F9" t="n">
-        <v>0</v>
+        <v>14189999</v>
       </c>
       <c r="G9" t="n">
-        <v>35297</v>
+        <v>14250000</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
@@ -904,7 +944,7 @@
         </is>
       </c>
       <c r="I9" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -913,12 +953,17 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Cucurbitacin biosynthetic gene cluster</t>
+          <t>Arabidopsis thaliana chromosome 5 sequence</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>cucurbitacin</t>
+          <t>tirucalla</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>
@@ -928,7 +973,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>BGC0001316</t>
+          <t>BGC0001315</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -943,14 +988,14 @@
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Lotus japonicus</t>
+          <t>Cucumis sativus</t>
         </is>
       </c>
       <c r="F10" t="n">
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>409731</v>
+        <v>35297</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
@@ -958,21 +1003,26 @@
         </is>
       </c>
       <c r="I10" t="n">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Terpene</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Linamarin / Lotaustralin biosynthetic gene cluster</t>
+          <t>Cucurbitacin biosynthetic gene cluster</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>linamarin,</t>
+          <t>cucurbitacin</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>
@@ -982,7 +1032,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>BGC0001317</t>
+          <t>BGC0001316</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -1004,7 +1054,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>277585</v>
+        <v>409731</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
@@ -1012,21 +1062,26 @@
         </is>
       </c>
       <c r="I11" t="n">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Lupeol biosynthetic gene cluster</t>
+          <t>Linamarin / Lotaustralin biosynthetic gene cluster</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>lupeol</t>
+          <t>linamarin,</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>
@@ -1036,7 +1091,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>BGC0001318</t>
+          <t>BGC0001317</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1051,14 +1106,14 @@
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Manihot esculenta</t>
+          <t>Lotus japonicus</t>
         </is>
       </c>
       <c r="F12" t="n">
         <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>80994</v>
+        <v>277585</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
@@ -1066,21 +1121,26 @@
         </is>
       </c>
       <c r="I12" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Terpene</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Linamarin / Lotaustralin biosynthetic gene cluster</t>
+          <t>Lupeol biosynthetic gene cluster</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>linamarin,</t>
+          <t>lupeol</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>
@@ -1090,7 +1150,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>BGC0001324</t>
+          <t>BGC0001318</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1105,14 +1165,14 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Solanum pimpinellifolium</t>
+          <t>Manihot esculenta</t>
         </is>
       </c>
       <c r="F13" t="n">
         <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>107124</v>
+        <v>80994</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
@@ -1120,21 +1180,26 @@
         </is>
       </c>
       <c r="I13" t="n">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>Other</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Solanum pimpinellifolium isolate LA1589 chromosome 8 terpene biosynthesis gene locus, partial sequence</t>
+          <t>Linamarin / Lotaustralin biosynthetic gene cluster</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>monoterpenes-diterpenes</t>
+          <t>linamarin,</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>
@@ -1144,7 +1209,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>BGC0001325</t>
+          <t>BGC0001321</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1159,14 +1224,14 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Papaver somniferum</t>
+          <t>Solanum habrochaites</t>
         </is>
       </c>
       <c r="F14" t="n">
         <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>401328</v>
+        <v>149366</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -1174,21 +1239,26 @@
         </is>
       </c>
       <c r="I14" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Alkaloid</t>
+          <t>Terpene</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Noscapine biosynthetic gene cluster</t>
+          <t>Solanum habrochaites isolate LA1778 chromosome 8 terpene biosynthesis gene locus, partial sequence</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>noscapine</t>
+          <t>monoterpenes-diterpenes</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>
@@ -1198,7 +1268,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>BGC0001756</t>
+          <t>BGC0001322</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1213,14 +1283,14 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana</t>
+          <t>Solanum lycopersicum</t>
         </is>
       </c>
       <c r="F15" t="n">
-        <v>4863612</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>4887487</v>
+        <v>127509</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -1228,7 +1298,7 @@
         </is>
       </c>
       <c r="I15" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1237,12 +1307,17 @@
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana chromosome 3, partial sequence</t>
+          <t>Solanum lycopersicum chromosome 8 terpene biosythesis gene locus, partial sequence</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>arathanatriene,</t>
+          <t>lycosantalonol</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.0</t>
         </is>
       </c>
     </row>
@@ -1252,7 +1327,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>BGC0001799</t>
+          <t>BGC0001323</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1267,14 +1342,14 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Papaver somniferum</t>
+          <t>Solanum pennellii</t>
         </is>
       </c>
       <c r="F16" t="n">
-        <v>78651</v>
+        <v>0</v>
       </c>
       <c r="G16" t="n">
-        <v>1013747</v>
+        <v>76813</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -1282,21 +1357,26 @@
         </is>
       </c>
       <c r="I16" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Alkaloid</t>
+          <t>Terpene</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>UNVERIFIED: Papaver somniferum (S)-reticuline epimerase-like (REPI1), REPI2, salutaridine synthase (SalSyn1), O-methyltransferase-1, SalSyn2, O-methyltransferase-2, salutaridinol 7-O-acetyltransferase (SalAT2), salutaridine reductase-like (SalR2), and thebaine synthase 2 (THS2) genes, partial sequence; thebaine synthase 1-like (THS1) gene, complete sequence; and SalR1 and SalAT1 genes, partial sequence</t>
+          <t>Solanum pennellii isolate LA0716 chromosome 8 terpene biosynthesis gene locus, partial sequence</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>thebaine</t>
+          <t>monoterpenes-diterpenes</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.0</t>
         </is>
       </c>
     </row>
@@ -1306,7 +1386,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>BGC0001997</t>
+          <t>BGC0001324</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1321,14 +1401,14 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Nicotiana tabacum</t>
+          <t>Solanum pimpinellifolium</t>
         </is>
       </c>
       <c r="F17" t="n">
-        <v>469295</v>
+        <v>0</v>
       </c>
       <c r="G17" t="n">
-        <v>543944</v>
+        <v>107124</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1345,12 +1425,17 @@
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Nicotiana tabacum cultivar K326 Nitab4.5_0001461, whole genome shotgun sequence</t>
+          <t>Solanum pimpinellifolium isolate LA1589 chromosome 8 terpene biosynthesis gene locus, partial sequence</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>capsidiol</t>
+          <t>monoterpenes-diterpenes</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>
@@ -1360,7 +1445,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>BGC0002389</t>
+          <t>BGC0001325</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1375,14 +1460,14 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Zea mays</t>
+          <t>Papaver somniferum</t>
         </is>
       </c>
       <c r="F18" t="n">
-        <v>56565232</v>
+        <v>0</v>
       </c>
       <c r="G18" t="n">
-        <v>56847613</v>
+        <v>401328</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1390,21 +1475,26 @@
         </is>
       </c>
       <c r="I18" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>Alkaloid</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Zea mays cultivar B73 chromosome 10, Zm-B73-REFERENCE-NAM-5.0, whole genome shotgun sequence</t>
+          <t>Noscapine biosynthetic gene cluster</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>β-bisabolene,</t>
+          <t>noscapine</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>
@@ -1414,7 +1504,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>BGC0002390</t>
+          <t>BGC0001756</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1429,14 +1519,14 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Zea mays</t>
+          <t>Arabidopsis thaliana</t>
         </is>
       </c>
       <c r="F19" t="n">
-        <v>33367131</v>
+        <v>4863612</v>
       </c>
       <c r="G19" t="n">
-        <v>34010443</v>
+        <v>4887487</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1444,7 +1534,7 @@
         </is>
       </c>
       <c r="I19" t="n">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1453,12 +1543,17 @@
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Zea mays cultivar B73 chromosome 5, Zm-B73-REFERENCE-NAM-5.0, whole genome shotgun sequence</t>
+          <t>Arabidopsis thaliana chromosome 3, partial sequence</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>zealexin</t>
+          <t>arathanatriene,</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>
@@ -1468,7 +1563,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>BGC0002391</t>
+          <t>BGC0001799</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1483,14 +1578,14 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Zea mays</t>
+          <t>Papaver somniferum</t>
         </is>
       </c>
       <c r="F20" t="n">
-        <v>285583113</v>
+        <v>78651</v>
       </c>
       <c r="G20" t="n">
-        <v>285654925</v>
+        <v>1013747</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1498,21 +1593,26 @@
         </is>
       </c>
       <c r="I20" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>Alkaloid</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>Zea mays cultivar B73 chromosome 1, Zm-B73-REFERENCE-NAM-5.0, whole genome shotgun sequence</t>
+          <t>UNVERIFIED: Papaver somniferum (S)-reticuline epimerase-like (REPI1), REPI2, salutaridine synthase (SalSyn1), O-methyltransferase-1, SalSyn2, O-methyltransferase-2, salutaridinol 7-O-acetyltransferase (SalAT2), salutaridine reductase-like (SalR2), and thebaine synthase 2 (THS2) genes, partial sequence; thebaine synthase 1-like (THS1) gene, complete sequence; and SalR1 and SalAT1 genes, partial sequence</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>zealexin</t>
+          <t>thebaine</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>
@@ -1522,7 +1622,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>BGC0002392</t>
+          <t>BGC0001997</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1537,14 +1637,14 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Oryza sativa Japonica Group</t>
+          <t>Nicotiana tabacum</t>
         </is>
       </c>
       <c r="F21" t="n">
-        <v>6494479</v>
+        <v>469295</v>
       </c>
       <c r="G21" t="n">
-        <v>6634480</v>
+        <v>543944</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1552,7 +1652,7 @@
         </is>
       </c>
       <c r="I21" t="n">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1561,12 +1661,17 @@
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Oryza sativa Japonica Group DNA, chromosome 7, cultivar: Nipponbare, complete sequence</t>
+          <t>Nicotiana tabacum cultivar K326 Nitab4.5_0001461, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>5,10-diketo-casbene</t>
+          <t>capsidiol</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>
@@ -1576,7 +1681,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>BGC0002393</t>
+          <t>BGC0002388</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1591,14 +1696,14 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Ricinus communis</t>
+          <t>Oryza sativa Japonica Group</t>
         </is>
       </c>
       <c r="F22" t="n">
-        <v>264511</v>
+        <v>21662581</v>
       </c>
       <c r="G22" t="n">
-        <v>337591</v>
+        <v>21906232</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
@@ -1606,7 +1711,7 @@
         </is>
       </c>
       <c r="I22" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1615,12 +1720,17 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Ricinus communis genomic scaffold scf_1106159296192, whole genome shotgun sequence</t>
+          <t>Oryza sativa Japonica Group DNA, chromosome 2, cultivar: Nipponbare, complete sequence</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>5a-hydroxy-casbene,</t>
+          <t>oryzalides,</t>
+        </is>
+      </c>
+      <c r="M22" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.0</t>
         </is>
       </c>
     </row>
@@ -1630,7 +1740,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>BGC0002394</t>
+          <t>BGC0002389</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1645,14 +1755,14 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Taxus chinensis</t>
+          <t>Zea mays</t>
         </is>
       </c>
       <c r="F23" t="n">
-        <v>55305454</v>
+        <v>56565232</v>
       </c>
       <c r="G23" t="n">
-        <v>55566904</v>
+        <v>56847613</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -1660,7 +1770,7 @@
         </is>
       </c>
       <c r="I23" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1669,12 +1779,17 @@
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Taxus chinensis isolate Ta-2019 chromosome 9, whole genome shotgun sequence</t>
+          <t>Zea mays cultivar B73 chromosome 10, Zm-B73-REFERENCE-NAM-5.0, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>taxa-4(20),11(12)-diene,</t>
+          <t>β-bisabolene,</t>
+        </is>
+      </c>
+      <c r="M23" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>
@@ -1684,7 +1799,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>BGC0002395</t>
+          <t>BGC0002390</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1699,14 +1814,14 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>Hordeum vulgare subsp. vulgare</t>
+          <t>Zea mays</t>
         </is>
       </c>
       <c r="F24" t="n">
-        <v>9581241</v>
+        <v>33367131</v>
       </c>
       <c r="G24" t="n">
-        <v>10180879</v>
+        <v>34010443</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -1714,7 +1829,7 @@
         </is>
       </c>
       <c r="I24" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1723,12 +1838,17 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Hordeum vulgare subsp. vulgare chromosome 2H, MorexV3_pseudomolecules_assembly, whole genome shotgun sequence</t>
+          <t>Zea mays cultivar B73 chromosome 5, Zm-B73-REFERENCE-NAM-5.0, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>11-hydroxy-hordetriene,</t>
+          <t>zealexin</t>
+        </is>
+      </c>
+      <c r="M24" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>
@@ -1738,7 +1858,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>BGC0002404</t>
+          <t>BGC0002391</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1753,14 +1873,14 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Solanum lycopersicum</t>
+          <t>Zea mays</t>
         </is>
       </c>
       <c r="F25" t="n">
-        <v>68007492</v>
+        <v>285583113</v>
       </c>
       <c r="G25" t="n">
-        <v>68031028</v>
+        <v>285654925</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
@@ -1768,21 +1888,26 @@
         </is>
       </c>
       <c r="I25" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Terpene</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Solanum lycopersicum cultivar Heinz 1706 chromosome 12, SL3.0, whole genome shotgun sequence</t>
+          <t>Zea mays cultivar B73 chromosome 1, Zm-B73-REFERENCE-NAM-5.0, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>falcarindiol</t>
+          <t>zealexin</t>
+        </is>
+      </c>
+      <c r="M25" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>
@@ -1792,7 +1917,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BGC0002405</t>
+          <t>BGC0002392</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1807,14 +1932,14 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Solanum lycopersicum</t>
+          <t>Oryza sativa Japonica Group</t>
         </is>
       </c>
       <c r="F26" t="n">
-        <v>57739269</v>
+        <v>6494479</v>
       </c>
       <c r="G26" t="n">
-        <v>57782130</v>
+        <v>6634480</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
@@ -1822,21 +1947,26 @@
         </is>
       </c>
       <c r="I26" t="n">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Saccharide</t>
+          <t>Terpene</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Solanum lycopersicum cultivar Heinz 1706 chromosome 7, SL3.0, whole genome shotgun sequence</t>
+          <t>Oryza sativa Japonica Group DNA, chromosome 7, cultivar: Nipponbare, complete sequence</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>mid-chain</t>
+          <t>5,10-diketo-casbene</t>
+        </is>
+      </c>
+      <c r="M26" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>
@@ -1846,7 +1976,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>BGC0002406</t>
+          <t>BGC0002393</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1861,14 +1991,14 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Oryza sativa Japonica Group</t>
+          <t>Ricinus communis</t>
         </is>
       </c>
       <c r="F27" t="n">
-        <v>12067615</v>
+        <v>264511</v>
       </c>
       <c r="G27" t="n">
-        <v>12262361</v>
+        <v>337591</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -1880,17 +2010,22 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Terpene</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Oryza sativa Japonica Group DNA, chromosome 10, cultivar: Nipponbare, complete sequence</t>
+          <t>Ricinus communis genomic scaffold scf_1106159296192, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>hydroxycinnamoyltyramine</t>
+          <t>5a-hydroxy-casbene,</t>
+        </is>
+      </c>
+      <c r="M27" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>
@@ -1900,7 +2035,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>BGC0002622</t>
+          <t>BGC0002394</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1915,14 +2050,14 @@
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Oryza sativa Japonica Group</t>
+          <t>Taxus chinensis</t>
         </is>
       </c>
       <c r="F28" t="n">
-        <v>21409012</v>
+        <v>55305454</v>
       </c>
       <c r="G28" t="n">
-        <v>21465464</v>
+        <v>55566904</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
@@ -1930,21 +2065,26 @@
         </is>
       </c>
       <c r="I28" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>Terpene</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Oryza sativa Japonica Group DNA, chromosome 9, cultivar: Nipponbare, complete sequence</t>
+          <t>Taxus chinensis isolate Ta-2019 chromosome 9, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>hydroxycinnamoylputrescine</t>
+          <t>taxa-4(20),11(12)-diene,</t>
+        </is>
+      </c>
+      <c r="M28" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>
@@ -1954,7 +2094,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>BGC0002721</t>
+          <t>BGC0002395</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1973,10 +2113,10 @@
         </is>
       </c>
       <c r="F29" t="n">
-        <v>17320184</v>
+        <v>9581241</v>
       </c>
       <c r="G29" t="n">
-        <v>17862889</v>
+        <v>10180879</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
@@ -1984,21 +2124,26 @@
         </is>
       </c>
       <c r="I29" t="n">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Saccharide</t>
+          <t>Terpene</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Hordeum vulgare subsp. vulgare chromosome 1H, MorexV3_pseudomolecules_assembly, whole genome shotgun sequence</t>
+          <t>Hordeum vulgare subsp. vulgare chromosome 2H, MorexV3_pseudomolecules_assembly, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>α-hydroxynitrile</t>
+          <t>11-hydroxy-hordetriene,</t>
+        </is>
+      </c>
+      <c r="M29" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>
@@ -2008,7 +2153,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>BGC0002722</t>
+          <t>BGC0002396</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -2023,14 +2168,14 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Saccharide</t>
+          <t>Salvia splendens</t>
         </is>
       </c>
       <c r="F30" t="n">
-        <v>1123004</v>
+        <v>21876301</v>
       </c>
       <c r="G30" t="n">
-        <v>1460949</v>
+        <v>21905825</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
@@ -2038,21 +2183,26 @@
         </is>
       </c>
       <c r="I30" t="n">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Alkaloid</t>
+          <t>Terpene</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Solanum tuberosum cultivar DM 1-3 516 R44 unplaced genomic scaffold, SolTub_3.0 scf00140, whole genome shotgun sequence</t>
+          <t>Salvia splendens isolate huo1 chromosome 20, whole genome shotgun sequence</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>α-chaconine,</t>
+          <t>tanshinones</t>
+        </is>
+      </c>
+      <c r="M30" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.0</t>
         </is>
       </c>
     </row>
@@ -2062,7 +2212,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>BGC0002723</t>
+          <t>BGC0002397</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
@@ -2077,14 +2227,14 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>Jatropha curcas</t>
+          <t>Arabidopsis thaliana</t>
         </is>
       </c>
       <c r="F31" t="n">
-        <v>7856</v>
+        <v>13032305</v>
       </c>
       <c r="G31" t="n">
-        <v>18675</v>
+        <v>13049106</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
@@ -2092,7 +2242,7 @@
         </is>
       </c>
       <c r="I31" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -2101,12 +2251,17 @@
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Jatropha curcas isolate ELGS0001-1231 unplaced genomic scaffold, RJC1_Hi-C scaffold_928, whole genome shotgun sequence</t>
+          <t>Arabidopsis thaliana chromosome 3, partial sequence</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>casbene</t>
+          <t>astallatene</t>
+        </is>
+      </c>
+      <c r="M31" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.0</t>
         </is>
       </c>
     </row>
@@ -2116,51 +2271,823 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
+          <t>BGC0002398</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Arabidopsis thaliana</t>
+        </is>
+      </c>
+      <c r="F32" t="n">
+        <v>11302430</v>
+      </c>
+      <c r="G32" t="n">
+        <v>11312823</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I32" t="n">
+        <v>3</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>Arabidopsis thaliana chromosome 3, partial sequence</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>ent-quiannuatene</t>
+        </is>
+      </c>
+      <c r="M32" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="1" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>BGC0002399</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Capsella rubella</t>
+        </is>
+      </c>
+      <c r="F33" t="n">
+        <v>4991784</v>
+      </c>
+      <c r="G33" t="n">
+        <v>5003638</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I33" t="n">
+        <v>4</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>Capsella rubella cultivar Monte Gargano unplaced genomic scaffold scaffold_3, whole genome shotgun sequence</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>caprutriene</t>
+        </is>
+      </c>
+      <c r="M33" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="1" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>BGC0002400</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Brassica oleracea var. oleracea</t>
+        </is>
+      </c>
+      <c r="F34" t="n">
+        <v>40080952</v>
+      </c>
+      <c r="G34" t="n">
+        <v>40133535</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I34" t="n">
+        <v>4</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>Brassica oleracea var. oleracea cultivar TO1000 chromosome C5, BOL, whole genome shotgun sequence</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>boleracene</t>
+        </is>
+      </c>
+      <c r="M34" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="1" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>BGC0002401</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Arabidopsis thaliana</t>
+        </is>
+      </c>
+      <c r="F35" t="n">
+        <v>19428887</v>
+      </c>
+      <c r="G35" t="n">
+        <v>19461706</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I35" t="n">
+        <v>10</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>Arabidopsis thaliana chromosome 3, partial sequence</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>euphol</t>
+        </is>
+      </c>
+      <c r="M35" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="1" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>BGC0002402</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>Spinacia oleracea</t>
+        </is>
+      </c>
+      <c r="F36" t="n">
+        <v>6310</v>
+      </c>
+      <c r="G36" t="n">
+        <v>44201</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I36" t="n">
+        <v>5</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>Spinacia oleracea cultivar SynViroflay unplaced genomic scaffold scaffold19898, whole genome shotgun sequence</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>yossosides</t>
+        </is>
+      </c>
+      <c r="M36" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>BGC0002403</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Hordeum vulgare subsp. vulgare</t>
+        </is>
+      </c>
+      <c r="F37" t="n">
+        <v>21755</v>
+      </c>
+      <c r="G37" t="n">
+        <v>151180</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I37" t="n">
+        <v>4</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Polyketide</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>Hordeum vulgare subsp. vulgare clone BAC 66C06, complete sequence</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>β-Diketones</t>
+        </is>
+      </c>
+      <c r="M37" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.0</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="1" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>BGC0002404</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>Solanum lycopersicum</t>
+        </is>
+      </c>
+      <c r="F38" t="n">
+        <v>68007492</v>
+      </c>
+      <c r="G38" t="n">
+        <v>68031028</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I38" t="n">
+        <v>3</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>Solanum lycopersicum cultivar Heinz 1706 chromosome 12, SL3.0, whole genome shotgun sequence</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>falcarindiol</t>
+        </is>
+      </c>
+      <c r="M38" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" s="1" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>BGC0002405</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Solanum lycopersicum</t>
+        </is>
+      </c>
+      <c r="F39" t="n">
+        <v>57739269</v>
+      </c>
+      <c r="G39" t="n">
+        <v>57782130</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I39" t="n">
+        <v>5</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>Saccharide</t>
+        </is>
+      </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>Solanum lycopersicum cultivar Heinz 1706 chromosome 7, SL3.0, whole genome shotgun sequence</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>mid-chain</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" s="1" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>BGC0002406</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Oryza sativa Japonica Group</t>
+        </is>
+      </c>
+      <c r="F40" t="n">
+        <v>12067615</v>
+      </c>
+      <c r="G40" t="n">
+        <v>12262361</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I40" t="n">
+        <v>17</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>Oryza sativa Japonica Group DNA, chromosome 10, cultivar: Nipponbare, complete sequence</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>hydroxycinnamoyltyramine</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" s="1" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>BGC0002622</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>Oryza sativa Japonica Group</t>
+        </is>
+      </c>
+      <c r="F41" t="n">
+        <v>21409012</v>
+      </c>
+      <c r="G41" t="n">
+        <v>21465464</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I41" t="n">
+        <v>3</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>Oryza sativa Japonica Group DNA, chromosome 9, cultivar: Nipponbare, complete sequence</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>hydroxycinnamoylputrescine</t>
+        </is>
+      </c>
+      <c r="M41" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>BGC0002721</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Hordeum vulgare subsp. vulgare</t>
+        </is>
+      </c>
+      <c r="F42" t="n">
+        <v>17320184</v>
+      </c>
+      <c r="G42" t="n">
+        <v>17862889</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I42" t="n">
+        <v>5</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>Saccharide</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>Hordeum vulgare subsp. vulgare chromosome 1H, MorexV3_pseudomolecules_assembly, whole genome shotgun sequence</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>α-hydroxynitrile</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" s="1" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>BGC0002722</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>Saccharide</t>
+        </is>
+      </c>
+      <c r="F43" t="n">
+        <v>1123004</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1460949</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I43" t="n">
+        <v>22</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>Alkaloid</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>Solanum tuberosum cultivar DM 1-3 516 R44 unplaced genomic scaffold, SolTub_3.0 scf00140, whole genome shotgun sequence</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>α-chaconine,</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" s="1" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>BGC0002723</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>Jatropha curcas</t>
+        </is>
+      </c>
+      <c r="F44" t="n">
+        <v>7856</v>
+      </c>
+      <c r="G44" t="n">
+        <v>18675</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I44" t="n">
+        <v>2</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>Jatropha curcas isolate ELGS0001-1231 unplaced genomic scaffold, RJC1_Hi-C scaffold_928, whole genome shotgun sequence</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>casbene</t>
+        </is>
+      </c>
+      <c r="M44" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
           <t>BGC0002724</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
         <is>
           <t>Jatropha curcas</t>
         </is>
       </c>
-      <c r="F32" t="n">
+      <c r="F45" t="n">
         <v>848628</v>
       </c>
-      <c r="G32" t="n">
+      <c r="G45" t="n">
         <v>912207</v>
       </c>
-      <c r="H32" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I32" t="n">
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>None</t>
+        </is>
+      </c>
+      <c r="I45" t="n">
         <v>6</v>
       </c>
-      <c r="J32" t="inlineStr">
+      <c r="J45" t="inlineStr">
         <is>
           <t>Terpene</t>
         </is>
       </c>
-      <c r="K32" t="inlineStr">
+      <c r="K45" t="inlineStr">
         <is>
           <t>Jatropha curcas isolate ELGS0001-1231 unplaced genomic scaffold, RJC1_Hi-C scaffold_989, whole genome shotgun sequence</t>
         </is>
       </c>
-      <c r="L32" t="inlineStr">
+      <c r="L45" t="inlineStr">
         <is>
           <t>casbene</t>
+        </is>
+      </c>
+      <c r="M45" t="inlineStr">
+        <is>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
getting publications from json
</commit_message>
<xml_diff>
--- a/general_data/mgc_plant_clusters.xlsx
+++ b/general_data/mgc_plant_clusters.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:N45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -494,6 +494,11 @@
           <t>mibig_version</t>
         </is>
       </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>publications</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -553,6 +558,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>['pubmed:21876149', 'pubmed:22882494']</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -612,6 +622,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>['pubmed:18356490']</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -671,6 +686,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>['pubmed:17872948']</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -730,6 +750,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>['pubmed:21985968', 'pubmed:19825834', 'doi:10.1105/tpc.108.063677']</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -789,6 +814,11 @@
           <t>mibig_gbk_3.0</t>
         </is>
       </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>['pubmed:21707799']</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -848,6 +878,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>['pubmed:11851909', 'pubmed:12620350', 'pubmed:18192444']</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -907,6 +942,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>['pubmed:23570231']</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -966,6 +1006,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>['pubmed:25502595']</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1025,6 +1070,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>['pubmed:25502595']</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1084,6 +1134,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>['pubmed:21707799']</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1143,6 +1198,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>['pubmed:23909862']</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1202,6 +1262,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>['pubmed:21707799']</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -1261,6 +1326,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>['pubmed:23757397']</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -1320,6 +1390,11 @@
           <t>mibig_gbk_3.0</t>
         </is>
       </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>['pubmed:23757397']</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -1379,6 +1454,11 @@
           <t>mibig_gbk_3.0</t>
         </is>
       </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>['pubmed:23757397']</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -1438,6 +1518,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>['pubmed:23757397']</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -1497,6 +1582,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>['pubmed:22653730']</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -1556,6 +1646,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>['pubmed:28673978']</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -1615,6 +1710,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>['pubmed:29807982']</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -1674,6 +1774,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>['doi:10.1007/s00425-019-03255-7']</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -1733,6 +1838,11 @@
           <t>mibig_gbk_3.0</t>
         </is>
       </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>['pubmed:19825834', 'doi:10.1105/tpc.108.063677']</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -1792,6 +1902,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>['pubmed:33106639']</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -1851,6 +1966,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>['pubmed:33106639']</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -1910,6 +2030,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>['pubmed:33106639']</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -1969,6 +2094,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>['pubmed:33328597', 'doi:10.1038/s41477-020-00816-7', 'doi:10.1111/nph.17406']</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -2028,6 +2158,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>['pubmed:25172144', 'doi:10.1105/tpc.114.129668']</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -2087,6 +2222,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>['pubmed:34267359']</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -2146,6 +2286,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>['doi:10.1101/2021.05.21.445084']</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -2205,6 +2350,11 @@
           <t>mibig_gbk_3.0</t>
         </is>
       </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>['pubmed:33514704']</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -2264,6 +2414,11 @@
           <t>mibig_gbk_3.0</t>
         </is>
       </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>['pubmed:28673978', 'doi:10.1073/pnas.1705567114']</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -2323,6 +2478,11 @@
           <t>mibig_gbk_3.0</t>
         </is>
       </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>['pubmed:28673978', 'doi:10.1073/pnas.1705567114']</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -2382,6 +2542,11 @@
           <t>mibig_gbk_3.0</t>
         </is>
       </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>['pubmed:28673978', 'doi:10.1073/pnas.1705567114']</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -2441,6 +2606,11 @@
           <t>mibig_gbk_3.0</t>
         </is>
       </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>['pubmed:28673978', 'doi:10.1073/pnas.1705567114', 'doi:10.1126/science.aau6389']</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -2500,6 +2670,11 @@
           <t>mibig_gbk_3.0</t>
         </is>
       </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>['pubmed:31769874']</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -2559,6 +2734,11 @@
           <t>mibig_gbk_3.0</t>
         </is>
       </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>['pubmed:32424305']</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -2618,6 +2798,11 @@
           <t>mibig_gbk_3.0</t>
         </is>
       </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>['pubmed:27255931', 'doi:10.1093/jxb/erw105']</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -2677,6 +2862,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>['pubmed:31923394']</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -2736,6 +2926,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>['pubmed:32613943']</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -2795,6 +2990,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>['doi:10.1016/j.scib.2021.03.015']</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -2854,6 +3054,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>['doi:10.1016/j.scib.2021.06.014']</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -2913,6 +3118,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>['pubmed:27337134', 'doi:10.1111/tpj.13247']</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -2972,6 +3182,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>['pubmed:23788733', 'doi:10.1126/science.1240230']</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -3031,6 +3246,11 @@
           <t>mibig_gbk_3.1</t>
         </is>
       </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>['pubmed:25172144', 'doi:10.1105/tpc.114.129668']</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -3088,6 +3308,11 @@
       <c r="M45" t="inlineStr">
         <is>
           <t>mibig_gbk_3.1</t>
+        </is>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>['pubmed:25172144', 'doi:10.1105/tpc.114.129668']</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing bugs, adding logger, and getting compounds
</commit_message>
<xml_diff>
--- a/general_data/mgc_plant_clusters.xlsx
+++ b/general_data/mgc_plant_clusters.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N45"/>
+  <dimension ref="A1:O45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -441,62 +441,67 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>cluster_doi</t>
+          <t>accession</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>cluster_name</t>
+          <t>organism</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>organism</t>
+          <t>cluster_start</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>cluster_start</t>
+          <t>cluster_end</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>cluster_end</t>
+          <t>num_of_coding_sequences</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>cluster_genbank_link</t>
+          <t>bionsythetic_class</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>num_of_genes</t>
+          <t>description</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>bionsythetic_class</t>
+          <t>main_product</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>description</t>
+          <t>mibig_version</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>main_product</t>
+          <t>completeness</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>mibig_version</t>
+          <t>evidence</t>
         </is>
       </c>
       <c r="N1" s="1" t="inlineStr">
         <is>
           <t>publications</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>ido_notes</t>
         </is>
       </c>
     </row>
@@ -511,56 +516,61 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>NC_003076.8</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
           <t>Arabidopsis thaliana</t>
         </is>
       </c>
+      <c r="E2" t="n">
+        <v>17023646</v>
+      </c>
       <c r="F2" t="n">
-        <v>17023645</v>
+        <v>17058245</v>
       </c>
       <c r="G2" t="n">
-        <v>17058245</v>
+        <v>4</v>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>5</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>Arabidopsis thaliana chromosome 5 sequence</t>
+        </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['marneral']</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana chromosome 5 sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L2" t="inlineStr">
         <is>
-          <t>marneral</t>
+          <t>complete</t>
         </is>
       </c>
       <c r="M2" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.1</t>
+          <t>['Heterologous expression', 'Gene expression correlated with compound production']</t>
         </is>
       </c>
       <c r="N2" t="inlineStr">
         <is>
           <t>['pubmed:21876149', 'pubmed:22882494']</t>
+        </is>
+      </c>
+      <c r="O2" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -575,56 +585,61 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>NC_003076.8</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
           <t>Arabidopsis thaliana</t>
         </is>
       </c>
+      <c r="E3" t="n">
+        <v>19428888</v>
+      </c>
       <c r="F3" t="n">
-        <v>19428887</v>
+        <v>19461689</v>
       </c>
       <c r="G3" t="n">
-        <v>19461689</v>
+        <v>6</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>4</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>Arabidopsis thaliana chromosome 5 sequence</t>
+        </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['thaliandiol', 'thalianol']</t>
         </is>
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana chromosome 5 sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
         <is>
-          <t>thaliandiol,</t>
+          <t>complete</t>
         </is>
       </c>
       <c r="M3" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.1</t>
+          <t>['Knock-out studies', 'Heterologous expression', 'Gene expression correlated with compound production']</t>
         </is>
       </c>
       <c r="N3" t="inlineStr">
         <is>
           <t>['pubmed:18356490']</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -639,56 +654,57 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>AP008210.2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
           <t>Oryza sativa Japonica Group</t>
         </is>
       </c>
+      <c r="E4" t="n">
+        <v>5310457</v>
+      </c>
       <c r="F4" t="n">
-        <v>5310456</v>
+        <v>5479082</v>
       </c>
       <c r="G4" t="n">
-        <v>5479082</v>
+        <v>7</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
-        <v>7</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>Oryza sativa Japonica Group DNA, chromosome 4, complete sequence, cultivar: Nipponbare</t>
+        </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['momilactone']</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
         <is>
-          <t>Oryza sativa Japonica Group DNA, chromosome 4, complete sequence, cultivar: Nipponbare</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>momilactone</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
-        <is>
-          <t>mibig_gbk_3.1</t>
-        </is>
-      </c>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr">
         <is>
           <t>['pubmed:17872948']</t>
+        </is>
+      </c>
+      <c r="O4" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -703,56 +719,61 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>AP008208.2</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
           <t>Oryza sativa Japonica Group</t>
         </is>
       </c>
+      <c r="E5" t="n">
+        <v>22520469</v>
+      </c>
       <c r="F5" t="n">
-        <v>22520468</v>
+        <v>22764099</v>
       </c>
       <c r="G5" t="n">
-        <v>22764099</v>
+        <v>11</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I5" t="n">
-        <v>10</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>Oryza sativa Japonica Group DNA, chromosome 2, complete sequence, cultivar: Nipponbare</t>
+        </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['oryzalides', 'phytocassane']</t>
         </is>
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>Oryza sativa Japonica Group DNA, chromosome 2, complete sequence, cultivar: Nipponbare</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>oryzalides,</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.1</t>
+          <t>['Heterologous expression', 'Gene expression correlated with compound production', 'Enzymatic assays']</t>
         </is>
       </c>
       <c r="N5" t="inlineStr">
         <is>
           <t>['pubmed:21985968', 'pubmed:19825834', 'doi:10.1105/tpc.108.063677']</t>
+        </is>
+      </c>
+      <c r="O5" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -767,56 +788,57 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>CM000760.1</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
           <t>Sorghum bicolor</t>
         </is>
       </c>
+      <c r="E6" t="n">
+        <v>1058885</v>
+      </c>
       <c r="F6" t="n">
-        <v>1058884</v>
+        <v>1163330</v>
       </c>
       <c r="G6" t="n">
-        <v>1163330</v>
+        <v>5</v>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I6" t="n">
-        <v>5</v>
+          <t>Saccharide</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>Sorghum bicolor chromosome 1, whole genome shotgun sequence</t>
+        </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Saccharide</t>
+          <t>['dhurrin']</t>
         </is>
       </c>
       <c r="K6" t="inlineStr">
         <is>
-          <t>Sorghum bicolor chromosome 1, whole genome shotgun sequence</t>
+          <t>mibig_gbk_3.0</t>
         </is>
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>dhurrin</t>
-        </is>
-      </c>
-      <c r="M6" t="inlineStr">
-        <is>
-          <t>mibig_gbk_3.0</t>
-        </is>
-      </c>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M6" t="inlineStr"/>
       <c r="N6" t="inlineStr">
         <is>
           <t>['pubmed:21707799']</t>
+        </is>
+      </c>
+      <c r="O6" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -831,56 +853,57 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>CM000780.3</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
           <t>Zea mays</t>
         </is>
       </c>
+      <c r="E7" t="n">
+        <v>3003162</v>
+      </c>
       <c r="F7" t="n">
-        <v>3003161</v>
+        <v>3267368</v>
       </c>
       <c r="G7" t="n">
-        <v>3267368</v>
+        <v>17</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I7" t="n">
-        <v>8</v>
+          <t>Alkaloid</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>Zea mays cultivar B73 chromosome 4</t>
+        </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>Alkaloid</t>
+          <t>['benzoxazinone', 'DIMBOA']</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
         <is>
-          <t>Zea mays cultivar B73 chromosome 4</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>benzoxazinone</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
-        <is>
-          <t>mibig_gbk_3.1</t>
-        </is>
-      </c>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M7" t="inlineStr"/>
       <c r="N7" t="inlineStr">
         <is>
           <t>['pubmed:11851909', 'pubmed:12620350', 'pubmed:18192444']</t>
+        </is>
+      </c>
+      <c r="O7" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -895,56 +918,57 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>NC_003075.7</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
           <t>Arabidopsis thaliana</t>
         </is>
       </c>
+      <c r="E8" t="n">
+        <v>8730000</v>
+      </c>
       <c r="F8" t="n">
-        <v>8729999</v>
+        <v>8820000</v>
       </c>
       <c r="G8" t="n">
-        <v>8820000</v>
+        <v>30</v>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I8" t="n">
-        <v>18</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>Arabidopsis thaliana chromosome 4 sequence</t>
+        </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['arabidiol-baruol']</t>
         </is>
       </c>
       <c r="K8" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana chromosome 4 sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L8" t="inlineStr">
         <is>
-          <t>arabidiol-baruol</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
-        <is>
-          <t>mibig_gbk_3.1</t>
-        </is>
-      </c>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M8" t="inlineStr"/>
       <c r="N8" t="inlineStr">
         <is>
           <t>['pubmed:23570231']</t>
+        </is>
+      </c>
+      <c r="O8" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -959,56 +983,57 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>NC_003076.8</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
           <t>Arabidopsis thaliana</t>
         </is>
       </c>
+      <c r="E9" t="n">
+        <v>14190000</v>
+      </c>
       <c r="F9" t="n">
-        <v>14189999</v>
+        <v>14250000</v>
       </c>
       <c r="G9" t="n">
-        <v>14250000</v>
+        <v>19</v>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I9" t="n">
-        <v>14</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>Arabidopsis thaliana chromosome 5 sequence</t>
+        </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['tirucalla']</t>
         </is>
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana chromosome 5 sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L9" t="inlineStr">
         <is>
-          <t>tirucalla</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
-          <t>mibig_gbk_3.1</t>
-        </is>
-      </c>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M9" t="inlineStr"/>
       <c r="N9" t="inlineStr">
         <is>
           <t>['pubmed:25502595']</t>
+        </is>
+      </c>
+      <c r="O9" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1023,56 +1048,57 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>MIBIG.BGC0001315.1</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
           <t>Cucumis sativus</t>
         </is>
       </c>
+      <c r="E10" t="n">
+        <v>0</v>
+      </c>
       <c r="F10" t="n">
-        <v>0</v>
+        <v>35297</v>
       </c>
       <c r="G10" t="n">
-        <v>35297</v>
+        <v>6</v>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I10" t="n">
-        <v>6</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>Cucurbitacin biosynthetic gene cluster</t>
+        </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['cucurbitacin']</t>
         </is>
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Cucurbitacin biosynthetic gene cluster</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L10" t="inlineStr">
         <is>
-          <t>cucurbitacin</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
-          <t>mibig_gbk_3.1</t>
-        </is>
-      </c>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M10" t="inlineStr"/>
       <c r="N10" t="inlineStr">
         <is>
           <t>['pubmed:25502595']</t>
+        </is>
+      </c>
+      <c r="O10" t="inlineStr">
+        <is>
+          <t>['start calculated from gbk', 'end calculated from gbk']</t>
         </is>
       </c>
     </row>
@@ -1087,56 +1113,57 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>MIBIG.BGC0001316.1</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
           <t>Lotus japonicus</t>
         </is>
       </c>
+      <c r="E11" t="n">
+        <v>0</v>
+      </c>
       <c r="F11" t="n">
-        <v>0</v>
+        <v>409731</v>
       </c>
       <c r="G11" t="n">
-        <v>409731</v>
+        <v>24</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I11" t="n">
-        <v>24</v>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>Linamarin / Lotaustralin biosynthetic gene cluster</t>
+        </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>['linamarin', 'lotaustralin']</t>
         </is>
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Linamarin / Lotaustralin biosynthetic gene cluster</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L11" t="inlineStr">
         <is>
-          <t>linamarin,</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
-          <t>mibig_gbk_3.1</t>
-        </is>
-      </c>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M11" t="inlineStr"/>
       <c r="N11" t="inlineStr">
         <is>
           <t>['pubmed:21707799']</t>
+        </is>
+      </c>
+      <c r="O11" t="inlineStr">
+        <is>
+          <t>['start calculated from gbk', 'end calculated from gbk']</t>
         </is>
       </c>
     </row>
@@ -1151,56 +1178,57 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>MIBIG.BGC0001317.1</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
           <t>Lotus japonicus</t>
         </is>
       </c>
+      <c r="E12" t="n">
+        <v>0</v>
+      </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>277585</v>
       </c>
       <c r="G12" t="n">
-        <v>277585</v>
+        <v>18</v>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I12" t="n">
-        <v>18</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>Lupeol biosynthetic gene cluster</t>
+        </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['lupeol']</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
         <is>
-          <t>Lupeol biosynthetic gene cluster</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L12" t="inlineStr">
         <is>
-          <t>lupeol</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
-        <is>
-          <t>mibig_gbk_3.1</t>
-        </is>
-      </c>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M12" t="inlineStr"/>
       <c r="N12" t="inlineStr">
         <is>
           <t>['pubmed:23909862']</t>
+        </is>
+      </c>
+      <c r="O12" t="inlineStr">
+        <is>
+          <t>['start calculated from gbk', 'end calculated from gbk']</t>
         </is>
       </c>
     </row>
@@ -1215,56 +1243,57 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>MIBIG.BGC0001318.1</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
           <t>Manihot esculenta</t>
         </is>
       </c>
+      <c r="E13" t="n">
+        <v>0</v>
+      </c>
       <c r="F13" t="n">
-        <v>0</v>
+        <v>80994</v>
       </c>
       <c r="G13" t="n">
-        <v>80994</v>
+        <v>16</v>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I13" t="n">
-        <v>13</v>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>Linamarin / Lotaustralin biosynthetic gene cluster</t>
+        </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>['linamarin', 'lotaustralin']</t>
         </is>
       </c>
       <c r="K13" t="inlineStr">
         <is>
-          <t>Linamarin / Lotaustralin biosynthetic gene cluster</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L13" t="inlineStr">
         <is>
-          <t>linamarin,</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
-        <is>
-          <t>mibig_gbk_3.1</t>
-        </is>
-      </c>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr"/>
       <c r="N13" t="inlineStr">
         <is>
           <t>['pubmed:21707799']</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>['start calculated from gbk', 'end calculated from gbk']</t>
         </is>
       </c>
     </row>
@@ -1279,56 +1308,57 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>KC807998.1</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
           <t>Solanum habrochaites</t>
         </is>
       </c>
+      <c r="E14" t="n">
+        <v>0</v>
+      </c>
       <c r="F14" t="n">
-        <v>0</v>
+        <v>149366</v>
       </c>
       <c r="G14" t="n">
-        <v>149366</v>
+        <v>14</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I14" t="n">
-        <v>0</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>Solanum habrochaites isolate LA1778 chromosome 8 terpene biosynthesis gene locus, partial sequence</t>
+        </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['monoterpenes-diterpenes']</t>
         </is>
       </c>
       <c r="K14" t="inlineStr">
         <is>
-          <t>Solanum habrochaites isolate LA1778 chromosome 8 terpene biosynthesis gene locus, partial sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L14" t="inlineStr">
         <is>
-          <t>monoterpenes-diterpenes</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
-        <is>
-          <t>mibig_gbk_3.1</t>
-        </is>
-      </c>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M14" t="inlineStr"/>
       <c r="N14" t="inlineStr">
         <is>
           <t>['pubmed:23757397']</t>
+        </is>
+      </c>
+      <c r="O14" t="inlineStr">
+        <is>
+          <t>['start calculated from gbk', 'end calculated from gbk']</t>
         </is>
       </c>
     </row>
@@ -1343,56 +1373,57 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>KC807995.1</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
           <t>Solanum lycopersicum</t>
         </is>
       </c>
+      <c r="E15" t="n">
+        <v>0</v>
+      </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>127509</v>
       </c>
       <c r="G15" t="n">
-        <v>127509</v>
+        <v>15</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I15" t="n">
-        <v>0</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>Solanum lycopersicum chromosome 8 terpene biosythesis gene locus, partial sequence</t>
+        </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['lycosantalonol']</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
         <is>
-          <t>Solanum lycopersicum chromosome 8 terpene biosythesis gene locus, partial sequence</t>
+          <t>mibig_gbk_3.0</t>
         </is>
       </c>
       <c r="L15" t="inlineStr">
         <is>
-          <t>lycosantalonol</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
-        <is>
-          <t>mibig_gbk_3.0</t>
-        </is>
-      </c>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M15" t="inlineStr"/>
       <c r="N15" t="inlineStr">
         <is>
           <t>['pubmed:23757397']</t>
+        </is>
+      </c>
+      <c r="O15" t="inlineStr">
+        <is>
+          <t>['start calculated from gbk', 'end calculated from gbk']</t>
         </is>
       </c>
     </row>
@@ -1407,56 +1438,57 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>KC807997.1</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
           <t>Solanum pennellii</t>
         </is>
       </c>
+      <c r="E16" t="n">
+        <v>0</v>
+      </c>
       <c r="F16" t="n">
-        <v>0</v>
+        <v>76813</v>
       </c>
       <c r="G16" t="n">
-        <v>76813</v>
+        <v>9</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I16" t="n">
-        <v>0</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>Solanum pennellii isolate LA0716 chromosome 8 terpene biosynthesis gene locus, partial sequence</t>
+        </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['monoterpenes-diterpenes']</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
         <is>
-          <t>Solanum pennellii isolate LA0716 chromosome 8 terpene biosynthesis gene locus, partial sequence</t>
+          <t>mibig_gbk_3.0</t>
         </is>
       </c>
       <c r="L16" t="inlineStr">
         <is>
-          <t>monoterpenes-diterpenes</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
-        <is>
-          <t>mibig_gbk_3.0</t>
-        </is>
-      </c>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M16" t="inlineStr"/>
       <c r="N16" t="inlineStr">
         <is>
           <t>['pubmed:23757397']</t>
+        </is>
+      </c>
+      <c r="O16" t="inlineStr">
+        <is>
+          <t>['start calculated from gbk', 'end calculated from gbk']</t>
         </is>
       </c>
     </row>
@@ -1471,56 +1503,57 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>KC807996.1</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
           <t>Solanum pimpinellifolium</t>
         </is>
       </c>
+      <c r="E17" t="n">
+        <v>0</v>
+      </c>
       <c r="F17" t="n">
-        <v>0</v>
+        <v>107124</v>
       </c>
       <c r="G17" t="n">
-        <v>107124</v>
+        <v>14</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I17" t="n">
-        <v>0</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>Solanum pimpinellifolium isolate LA1589 chromosome 8 terpene biosynthesis gene locus, partial sequence</t>
+        </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['monoterpenes-diterpenes']</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
         <is>
-          <t>Solanum pimpinellifolium isolate LA1589 chromosome 8 terpene biosynthesis gene locus, partial sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L17" t="inlineStr">
         <is>
-          <t>monoterpenes-diterpenes</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
-        <is>
-          <t>mibig_gbk_3.1</t>
-        </is>
-      </c>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M17" t="inlineStr"/>
       <c r="N17" t="inlineStr">
         <is>
           <t>['pubmed:23757397']</t>
+        </is>
+      </c>
+      <c r="O17" t="inlineStr">
+        <is>
+          <t>['start calculated from gbk', 'end calculated from gbk']</t>
         </is>
       </c>
     </row>
@@ -1535,56 +1568,57 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>MIBIG.BGC0001325.1</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
           <t>Papaver somniferum</t>
         </is>
       </c>
+      <c r="E18" t="n">
+        <v>0</v>
+      </c>
       <c r="F18" t="n">
-        <v>0</v>
+        <v>401328</v>
       </c>
       <c r="G18" t="n">
-        <v>401328</v>
+        <v>10</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I18" t="n">
-        <v>10</v>
+          <t>Alkaloid</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>Noscapine biosynthetic gene cluster</t>
+        </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>Alkaloid</t>
+          <t>['noscapine']</t>
         </is>
       </c>
       <c r="K18" t="inlineStr">
         <is>
-          <t>Noscapine biosynthetic gene cluster</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L18" t="inlineStr">
         <is>
-          <t>noscapine</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
-        <is>
-          <t>mibig_gbk_3.1</t>
-        </is>
-      </c>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M18" t="inlineStr"/>
       <c r="N18" t="inlineStr">
         <is>
           <t>['pubmed:22653730']</t>
+        </is>
+      </c>
+      <c r="O18" t="inlineStr">
+        <is>
+          <t>['start calculated from gbk', 'end calculated from gbk']</t>
         </is>
       </c>
     </row>
@@ -1599,56 +1633,57 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>CP002686.1</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
           <t>Arabidopsis thaliana</t>
         </is>
       </c>
+      <c r="E19" t="n">
+        <v>4863613</v>
+      </c>
       <c r="F19" t="n">
-        <v>4863612</v>
+        <v>4887487</v>
       </c>
       <c r="G19" t="n">
-        <v>4887487</v>
+        <v>7</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I19" t="n">
-        <v>10</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>Arabidopsis thaliana chromosome 3, partial sequence</t>
+        </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['arathanatriene', 'retigeranin']</t>
         </is>
       </c>
       <c r="K19" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana chromosome 3, partial sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L19" t="inlineStr">
         <is>
-          <t>arathanatriene,</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
-        <is>
-          <t>mibig_gbk_3.1</t>
-        </is>
-      </c>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M19" t="inlineStr"/>
       <c r="N19" t="inlineStr">
         <is>
           <t>['pubmed:28673978']</t>
+        </is>
+      </c>
+      <c r="O19" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1663,56 +1698,57 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>MH011344.1</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
           <t>Papaver somniferum</t>
         </is>
       </c>
+      <c r="E20" t="n">
+        <v>78652</v>
+      </c>
       <c r="F20" t="n">
-        <v>78651</v>
+        <v>1013747</v>
       </c>
       <c r="G20" t="n">
-        <v>1013747</v>
+        <v>12</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I20" t="n">
-        <v>12</v>
+          <t>Alkaloid</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>UNVERIFIED: Papaver somniferum (S)-reticuline epimerase-like (REPI1), REPI2, salutaridine synthase (SalSyn1), O-methyltransferase-1, SalSyn2, O-methyltransferase-2, salutaridinol 7-O-acetyltransferase (SalAT2), salutaridine reductase-like (SalR2), and thebaine synthase 2 (THS2) genes, partial sequence; thebaine synthase 1-like (THS1) gene, complete sequence; and SalR1 and SalAT1 genes, partial sequence</t>
+        </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Alkaloid</t>
+          <t>['thebaine']</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
         <is>
-          <t>UNVERIFIED: Papaver somniferum (S)-reticuline epimerase-like (REPI1), REPI2, salutaridine synthase (SalSyn1), O-methyltransferase-1, SalSyn2, O-methyltransferase-2, salutaridinol 7-O-acetyltransferase (SalAT2), salutaridine reductase-like (SalR2), and thebaine synthase 2 (THS2) genes, partial sequence; thebaine synthase 1-like (THS1) gene, complete sequence; and SalR1 and SalAT1 genes, partial sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L20" t="inlineStr">
         <is>
-          <t>thebaine</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
-        <is>
-          <t>mibig_gbk_3.1</t>
-        </is>
-      </c>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M20" t="inlineStr"/>
       <c r="N20" t="inlineStr">
         <is>
           <t>['pubmed:29807982']</t>
+        </is>
+      </c>
+      <c r="O20" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1727,56 +1763,57 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>NCAA01001461.1</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
           <t>Nicotiana tabacum</t>
         </is>
       </c>
+      <c r="E21" t="n">
+        <v>469296</v>
+      </c>
       <c r="F21" t="n">
-        <v>469295</v>
+        <v>543944</v>
       </c>
       <c r="G21" t="n">
-        <v>543944</v>
+        <v>14</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I21" t="n">
-        <v>0</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>Nicotiana tabacum cultivar K326 Nitab4.5_0001461, whole genome shotgun sequence</t>
+        </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['capsidiol']</t>
         </is>
       </c>
       <c r="K21" t="inlineStr">
         <is>
-          <t>Nicotiana tabacum cultivar K326 Nitab4.5_0001461, whole genome shotgun sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L21" t="inlineStr">
         <is>
-          <t>capsidiol</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
-        <is>
-          <t>mibig_gbk_3.1</t>
-        </is>
-      </c>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M21" t="inlineStr"/>
       <c r="N21" t="inlineStr">
         <is>
           <t>['doi:10.1007/s00425-019-03255-7']</t>
+        </is>
+      </c>
+      <c r="O21" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1791,56 +1828,61 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>AP014958.1</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
           <t>Oryza sativa Japonica Group</t>
         </is>
       </c>
+      <c r="E22" t="n">
+        <v>21662582</v>
+      </c>
       <c r="F22" t="n">
-        <v>21662581</v>
+        <v>21906232</v>
       </c>
       <c r="G22" t="n">
-        <v>21906232</v>
+        <v>21</v>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I22" t="n">
-        <v>20</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>Oryza sativa Japonica Group DNA, chromosome 2, cultivar: Nipponbare, complete sequence</t>
+        </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['oryzalides', 'phytocassanes']</t>
         </is>
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Oryza sativa Japonica Group DNA, chromosome 2, cultivar: Nipponbare, complete sequence</t>
+          <t>mibig_gbk_3.0</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
         <is>
-          <t>oryzalides,</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M22" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.0</t>
+          <t>['Heterologous expression', 'Gene expression correlated with compound production', 'Enzymatic assays']</t>
         </is>
       </c>
       <c r="N22" t="inlineStr">
         <is>
           <t>['pubmed:19825834', 'doi:10.1105/tpc.108.063677']</t>
+        </is>
+      </c>
+      <c r="O22" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1855,56 +1897,61 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>GPC_000007952.1</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
           <t>Zea mays</t>
         </is>
       </c>
+      <c r="E23" t="n">
+        <v>56565233</v>
+      </c>
       <c r="F23" t="n">
-        <v>56565232</v>
+        <v>56847613</v>
       </c>
       <c r="G23" t="n">
-        <v>56847613</v>
+        <v>3</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I23" t="n">
-        <v>4</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>Zea mays cultivar B73 chromosome 10, Zm-B73-REFERENCE-NAM-5.0, whole genome shotgun sequence</t>
+        </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['β-bisabolene', 'β-macrocarpene']</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
         <is>
-          <t>Zea mays cultivar B73 chromosome 10, Zm-B73-REFERENCE-NAM-5.0, whole genome shotgun sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L23" t="inlineStr">
         <is>
-          <t>β-bisabolene,</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M23" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.1</t>
+          <t>['Heterologous expression', 'Gene expression correlated with compound production']</t>
         </is>
       </c>
       <c r="N23" t="inlineStr">
         <is>
           <t>['pubmed:33106639']</t>
+        </is>
+      </c>
+      <c r="O23" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1919,56 +1966,61 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>GPC_000007947.1</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
           <t>Zea mays</t>
         </is>
       </c>
+      <c r="E24" t="n">
+        <v>33367132</v>
+      </c>
       <c r="F24" t="n">
-        <v>33367131</v>
+        <v>34010443</v>
       </c>
       <c r="G24" t="n">
-        <v>34010443</v>
+        <v>19</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I24" t="n">
-        <v>14</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>Zea mays cultivar B73 chromosome 5, Zm-B73-REFERENCE-NAM-5.0, whole genome shotgun sequence</t>
+        </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['zealexin', 'A1']</t>
         </is>
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Zea mays cultivar B73 chromosome 5, Zm-B73-REFERENCE-NAM-5.0, whole genome shotgun sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L24" t="inlineStr">
         <is>
-          <t>zealexin</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M24" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.1</t>
+          <t>['Heterologous expression', 'Gene expression correlated with compound production']</t>
         </is>
       </c>
       <c r="N24" t="inlineStr">
         <is>
           <t>['pubmed:33106639']</t>
+        </is>
+      </c>
+      <c r="O24" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -1983,56 +2035,61 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>GPC_000007943.1</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
           <t>Zea mays</t>
         </is>
       </c>
+      <c r="E25" t="n">
+        <v>285583114</v>
+      </c>
       <c r="F25" t="n">
-        <v>285583113</v>
+        <v>285654925</v>
       </c>
       <c r="G25" t="n">
-        <v>285654925</v>
+        <v>2</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I25" t="n">
-        <v>2</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>Zea mays cultivar B73 chromosome 1, Zm-B73-REFERENCE-NAM-5.0, whole genome shotgun sequence</t>
+        </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['zealexin', 'B2', 'zealexin', 'C2']</t>
         </is>
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>Zea mays cultivar B73 chromosome 1, Zm-B73-REFERENCE-NAM-5.0, whole genome shotgun sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
         <is>
-          <t>zealexin</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M25" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.1</t>
+          <t>['Heterologous expression', 'Gene expression correlated with compound production']</t>
         </is>
       </c>
       <c r="N25" t="inlineStr">
         <is>
           <t>['pubmed:33106639']</t>
+        </is>
+      </c>
+      <c r="O25" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2047,56 +2104,61 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>AP014963.1</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
           <t>Oryza sativa Japonica Group</t>
         </is>
       </c>
+      <c r="E26" t="n">
+        <v>6494480</v>
+      </c>
       <c r="F26" t="n">
-        <v>6494479</v>
+        <v>6634480</v>
       </c>
       <c r="G26" t="n">
-        <v>6634480</v>
+        <v>16</v>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I26" t="n">
-        <v>16</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>Oryza sativa Japonica Group DNA, chromosome 7, cultivar: Nipponbare, complete sequence</t>
+        </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['5,10-diketo-casbene']</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
         <is>
-          <t>Oryza sativa Japonica Group DNA, chromosome 7, cultivar: Nipponbare, complete sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L26" t="inlineStr">
         <is>
-          <t>5,10-diketo-casbene</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M26" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.1</t>
+          <t>['Enzymatic assays']</t>
         </is>
       </c>
       <c r="N26" t="inlineStr">
         <is>
           <t>['pubmed:33328597', 'doi:10.1038/s41477-020-00816-7', 'doi:10.1111/nph.17406']</t>
+        </is>
+      </c>
+      <c r="O26" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2111,56 +2173,61 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>EQ973781.1</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
           <t>Ricinus communis</t>
         </is>
       </c>
+      <c r="E27" t="n">
+        <v>264512</v>
+      </c>
       <c r="F27" t="n">
-        <v>264511</v>
+        <v>337591</v>
       </c>
       <c r="G27" t="n">
-        <v>337591</v>
+        <v>17</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I27" t="n">
-        <v>17</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>Ricinus communis genomic scaffold scf_1106159296192, whole genome shotgun sequence</t>
+        </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['5a-hydroxy-casbene', '5-keto-7,8-epoxy-casbene', '5-keto-casbene', '5-keto-neocembrene', 'casbene', 'neocembrene']</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
         <is>
-          <t>Ricinus communis genomic scaffold scf_1106159296192, whole genome shotgun sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L27" t="inlineStr">
         <is>
-          <t>5a-hydroxy-casbene,</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M27" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.1</t>
+          <t>['Heterologous expression']</t>
         </is>
       </c>
       <c r="N27" t="inlineStr">
         <is>
           <t>['pubmed:25172144', 'doi:10.1105/tpc.114.129668']</t>
+        </is>
+      </c>
+      <c r="O27" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2175,56 +2242,61 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>CM034154.1</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
           <t>Taxus chinensis</t>
         </is>
       </c>
+      <c r="E28" t="n">
+        <v>55305455</v>
+      </c>
       <c r="F28" t="n">
-        <v>55305454</v>
+        <v>55566904</v>
       </c>
       <c r="G28" t="n">
-        <v>55566904</v>
+        <v>6</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I28" t="n">
-        <v>6</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>Taxus chinensis isolate Ta-2019 chromosome 9, whole genome shotgun sequence</t>
+        </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['taxa-4(20),11(12)-diene', 'taxa-4(5),11(12)-diene']</t>
         </is>
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>Taxus chinensis isolate Ta-2019 chromosome 9, whole genome shotgun sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
         <is>
-          <t>taxa-4(20),11(12)-diene,</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M28" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.1</t>
+          <t>['Heterologous expression', 'Gene expression correlated with compound production']</t>
         </is>
       </c>
       <c r="N28" t="inlineStr">
         <is>
           <t>['pubmed:34267359']</t>
+        </is>
+      </c>
+      <c r="O28" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2239,56 +2311,61 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>GPC_000011790.1</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
           <t>Hordeum vulgare subsp. vulgare</t>
         </is>
       </c>
+      <c r="E29" t="n">
+        <v>9581242</v>
+      </c>
       <c r="F29" t="n">
-        <v>9581241</v>
+        <v>10180879</v>
       </c>
       <c r="G29" t="n">
-        <v>10180879</v>
+        <v>14</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I29" t="n">
-        <v>19</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>Hordeum vulgare subsp. vulgare chromosome 2H, MorexV3_pseudomolecules_assembly, whole genome shotgun sequence</t>
+        </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['11-hydroxy-hordetriene', 'hordediene', 'hordetriene']</t>
         </is>
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>Hordeum vulgare subsp. vulgare chromosome 2H, MorexV3_pseudomolecules_assembly, whole genome shotgun sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
         <is>
-          <t>11-hydroxy-hordetriene,</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M29" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.1</t>
+          <t>['Heterologous expression', 'Enzymatic assays']</t>
         </is>
       </c>
       <c r="N29" t="inlineStr">
         <is>
           <t>['doi:10.1101/2021.05.21.445084']</t>
+        </is>
+      </c>
+      <c r="O29" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2303,56 +2380,61 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>CM031491.1</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E30" t="inlineStr">
-        <is>
           <t>Salvia splendens</t>
         </is>
       </c>
+      <c r="E30" t="n">
+        <v>21876302</v>
+      </c>
       <c r="F30" t="n">
-        <v>21876301</v>
+        <v>21905825</v>
       </c>
       <c r="G30" t="n">
-        <v>21905825</v>
+        <v>3</v>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I30" t="n">
-        <v>1</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>Salvia splendens isolate huo1 chromosome 20, whole genome shotgun sequence</t>
+        </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['tanshinones']</t>
         </is>
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>Salvia splendens isolate huo1 chromosome 20, whole genome shotgun sequence</t>
+          <t>mibig_gbk_3.0</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
         <is>
-          <t>tanshinones</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M30" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.0</t>
+          <t>['Heterologous expression', 'Enzymatic assays']</t>
         </is>
       </c>
       <c r="N30" t="inlineStr">
         <is>
           <t>['pubmed:33514704']</t>
+        </is>
+      </c>
+      <c r="O30" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2367,56 +2449,61 @@
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>CP002686.1</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
           <t>Arabidopsis thaliana</t>
         </is>
       </c>
+      <c r="E31" t="n">
+        <v>13032306</v>
+      </c>
       <c r="F31" t="n">
-        <v>13032305</v>
+        <v>13049106</v>
       </c>
       <c r="G31" t="n">
-        <v>13049106</v>
+        <v>2</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I31" t="n">
-        <v>4</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>Arabidopsis thaliana chromosome 3, partial sequence</t>
+        </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['astallatene']</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana chromosome 3, partial sequence</t>
+          <t>mibig_gbk_3.0</t>
         </is>
       </c>
       <c r="L31" t="inlineStr">
         <is>
-          <t>astallatene</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M31" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.0</t>
+          <t>['Heterologous expression']</t>
         </is>
       </c>
       <c r="N31" t="inlineStr">
         <is>
           <t>['pubmed:28673978', 'doi:10.1073/pnas.1705567114']</t>
+        </is>
+      </c>
+      <c r="O31" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2431,56 +2518,61 @@
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>CP002686.1</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
           <t>Arabidopsis thaliana</t>
         </is>
       </c>
+      <c r="E32" t="n">
+        <v>11302431</v>
+      </c>
       <c r="F32" t="n">
-        <v>11302430</v>
+        <v>11312823</v>
       </c>
       <c r="G32" t="n">
-        <v>11312823</v>
+        <v>3</v>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I32" t="n">
-        <v>3</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>Arabidopsis thaliana chromosome 3, partial sequence</t>
+        </is>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['ent-quiannuatene']</t>
         </is>
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana chromosome 3, partial sequence</t>
+          <t>mibig_gbk_3.0</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
         <is>
-          <t>ent-quiannuatene</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M32" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.0</t>
+          <t>['Heterologous expression']</t>
         </is>
       </c>
       <c r="N32" t="inlineStr">
         <is>
           <t>['pubmed:28673978', 'doi:10.1073/pnas.1705567114']</t>
+        </is>
+      </c>
+      <c r="O32" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2495,56 +2587,61 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>KB870807.1</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
           <t>Capsella rubella</t>
         </is>
       </c>
+      <c r="E33" t="n">
+        <v>4991785</v>
+      </c>
       <c r="F33" t="n">
-        <v>4991784</v>
+        <v>5003638</v>
       </c>
       <c r="G33" t="n">
-        <v>5003638</v>
+        <v>4</v>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I33" t="n">
-        <v>4</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>Capsella rubella cultivar Monte Gargano unplaced genomic scaffold scaffold_3, whole genome shotgun sequence</t>
+        </is>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['caprutriene']</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
         <is>
-          <t>Capsella rubella cultivar Monte Gargano unplaced genomic scaffold scaffold_3, whole genome shotgun sequence</t>
+          <t>mibig_gbk_3.0</t>
         </is>
       </c>
       <c r="L33" t="inlineStr">
         <is>
-          <t>caprutriene</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M33" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.0</t>
+          <t>['Heterologous expression']</t>
         </is>
       </c>
       <c r="N33" t="inlineStr">
         <is>
           <t>['pubmed:28673978', 'doi:10.1073/pnas.1705567114']</t>
+        </is>
+      </c>
+      <c r="O33" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2559,56 +2656,61 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>GPC_000001832.1</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
           <t>Brassica oleracea var. oleracea</t>
         </is>
       </c>
+      <c r="E34" t="n">
+        <v>40080953</v>
+      </c>
       <c r="F34" t="n">
-        <v>40080952</v>
+        <v>40133535</v>
       </c>
       <c r="G34" t="n">
-        <v>40133535</v>
+        <v>3</v>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I34" t="n">
-        <v>4</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>Brassica oleracea var. oleracea cultivar TO1000 chromosome C5, BOL, whole genome shotgun sequence</t>
+        </is>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['boleracene']</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
         <is>
-          <t>Brassica oleracea var. oleracea cultivar TO1000 chromosome C5, BOL, whole genome shotgun sequence</t>
+          <t>mibig_gbk_3.0</t>
         </is>
       </c>
       <c r="L34" t="inlineStr">
         <is>
-          <t>boleracene</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M34" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.0</t>
+          <t>['Heterologous expression']</t>
         </is>
       </c>
       <c r="N34" t="inlineStr">
         <is>
           <t>['pubmed:28673978', 'doi:10.1073/pnas.1705567114', 'doi:10.1126/science.aau6389']</t>
+        </is>
+      </c>
+      <c r="O34" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2623,56 +2725,61 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>CP002686.1</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
           <t>Arabidopsis thaliana</t>
         </is>
       </c>
+      <c r="E35" t="n">
+        <v>19428888</v>
+      </c>
       <c r="F35" t="n">
-        <v>19428887</v>
+        <v>19461706</v>
       </c>
       <c r="G35" t="n">
-        <v>19461706</v>
+        <v>9</v>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I35" t="n">
-        <v>10</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>Arabidopsis thaliana chromosome 3, partial sequence</t>
+        </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['euphol']</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
         <is>
-          <t>Arabidopsis thaliana chromosome 3, partial sequence</t>
+          <t>mibig_gbk_3.0</t>
         </is>
       </c>
       <c r="L35" t="inlineStr">
         <is>
-          <t>euphol</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M35" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.0</t>
+          <t>['Knock-out studies', 'Heterologous expression']</t>
         </is>
       </c>
       <c r="N35" t="inlineStr">
         <is>
           <t>['pubmed:31769874']</t>
+        </is>
+      </c>
+      <c r="O35" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2687,56 +2794,61 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>KQ150485.1</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
           <t>Spinacia oleracea</t>
         </is>
       </c>
+      <c r="E36" t="n">
+        <v>6311</v>
+      </c>
       <c r="F36" t="n">
-        <v>6310</v>
+        <v>44201</v>
       </c>
       <c r="G36" t="n">
-        <v>44201</v>
+        <v>5</v>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I36" t="n">
-        <v>5</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>Spinacia oleracea cultivar SynViroflay unplaced genomic scaffold scaffold19898, whole genome shotgun sequence</t>
+        </is>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['yossosides']</t>
         </is>
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Spinacia oleracea cultivar SynViroflay unplaced genomic scaffold scaffold19898, whole genome shotgun sequence</t>
+          <t>mibig_gbk_3.0</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
         <is>
-          <t>yossosides</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M36" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.0</t>
+          <t>['Knock-out studies', 'Heterologous expression']</t>
         </is>
       </c>
       <c r="N36" t="inlineStr">
         <is>
           <t>['pubmed:32424305']</t>
+        </is>
+      </c>
+      <c r="O36" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2751,56 +2863,61 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>KU721941.1</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
           <t>Hordeum vulgare subsp. vulgare</t>
         </is>
       </c>
+      <c r="E37" t="n">
+        <v>21756</v>
+      </c>
       <c r="F37" t="n">
-        <v>21755</v>
+        <v>151180</v>
       </c>
       <c r="G37" t="n">
-        <v>151180</v>
+        <v>4</v>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I37" t="n">
-        <v>4</v>
+          <t>Polyketide</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>Hordeum vulgare subsp. vulgare clone BAC 66C06, complete sequence</t>
+        </is>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Polyketide</t>
+          <t>['β-Diketones']</t>
         </is>
       </c>
       <c r="K37" t="inlineStr">
         <is>
-          <t>Hordeum vulgare subsp. vulgare clone BAC 66C06, complete sequence</t>
+          <t>mibig_gbk_3.0</t>
         </is>
       </c>
       <c r="L37" t="inlineStr">
         <is>
-          <t>β-Diketones</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M37" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.0</t>
+          <t>['Gene expression correlated with compound production']</t>
         </is>
       </c>
       <c r="N37" t="inlineStr">
         <is>
           <t>['pubmed:27255931', 'doi:10.1093/jxb/erw105']</t>
+        </is>
+      </c>
+      <c r="O37" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2815,56 +2932,61 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>GPC_000003970.1</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E38" t="inlineStr">
-        <is>
           <t>Solanum lycopersicum</t>
         </is>
       </c>
+      <c r="E38" t="n">
+        <v>68007493</v>
+      </c>
       <c r="F38" t="n">
-        <v>68007492</v>
+        <v>68031028</v>
       </c>
       <c r="G38" t="n">
-        <v>68031028</v>
+        <v>4</v>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I38" t="n">
-        <v>3</v>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>Solanum lycopersicum cultivar Heinz 1706 chromosome 12, SL3.0, whole genome shotgun sequence</t>
+        </is>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>['falcarindiol']</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
         <is>
-          <t>Solanum lycopersicum cultivar Heinz 1706 chromosome 12, SL3.0, whole genome shotgun sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L38" t="inlineStr">
         <is>
-          <t>falcarindiol</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M38" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.1</t>
+          <t>['Knock-out studies', 'Heterologous expression', 'Gene expression correlated with compound production']</t>
         </is>
       </c>
       <c r="N38" t="inlineStr">
         <is>
           <t>['pubmed:31923394']</t>
+        </is>
+      </c>
+      <c r="O38" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2879,56 +3001,57 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>GPC_000003965.1</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
           <t>Solanum lycopersicum</t>
         </is>
       </c>
+      <c r="E39" t="n">
+        <v>57739270</v>
+      </c>
       <c r="F39" t="n">
-        <v>57739269</v>
+        <v>57782130</v>
       </c>
       <c r="G39" t="n">
-        <v>57782130</v>
+        <v>4</v>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I39" t="n">
-        <v>5</v>
+          <t>Saccharide</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>Solanum lycopersicum cultivar Heinz 1706 chromosome 7, SL3.0, whole genome shotgun sequence</t>
+        </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>Saccharide</t>
+          <t>['mid-chain', 'acyl', 'sugars']</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Solanum lycopersicum cultivar Heinz 1706 chromosome 7, SL3.0, whole genome shotgun sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L39" t="inlineStr">
         <is>
-          <t>mid-chain</t>
-        </is>
-      </c>
-      <c r="M39" t="inlineStr">
-        <is>
-          <t>mibig_gbk_3.1</t>
-        </is>
-      </c>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M39" t="inlineStr"/>
       <c r="N39" t="inlineStr">
         <is>
           <t>['pubmed:32613943']</t>
+        </is>
+      </c>
+      <c r="O39" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -2943,56 +3066,57 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>AP014966.1</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
           <t>Oryza sativa Japonica Group</t>
         </is>
       </c>
+      <c r="E40" t="n">
+        <v>12067616</v>
+      </c>
       <c r="F40" t="n">
-        <v>12067615</v>
+        <v>12262361</v>
       </c>
       <c r="G40" t="n">
-        <v>12262361</v>
+        <v>20</v>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I40" t="n">
-        <v>17</v>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>Oryza sativa Japonica Group DNA, chromosome 10, cultivar: Nipponbare, complete sequence</t>
+        </is>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>['hydroxycinnamoyltyramine']</t>
         </is>
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>Oryza sativa Japonica Group DNA, chromosome 10, cultivar: Nipponbare, complete sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
         <is>
-          <t>hydroxycinnamoyltyramine</t>
-        </is>
-      </c>
-      <c r="M40" t="inlineStr">
-        <is>
-          <t>mibig_gbk_3.1</t>
-        </is>
-      </c>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M40" t="inlineStr"/>
       <c r="N40" t="inlineStr">
         <is>
           <t>['doi:10.1016/j.scib.2021.03.015']</t>
+        </is>
+      </c>
+      <c r="O40" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -3007,56 +3131,61 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>AP014965.1</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
           <t>Oryza sativa Japonica Group</t>
         </is>
       </c>
+      <c r="E41" t="n">
+        <v>21409013</v>
+      </c>
       <c r="F41" t="n">
-        <v>21409012</v>
+        <v>21465464</v>
       </c>
       <c r="G41" t="n">
-        <v>21465464</v>
+        <v>3</v>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I41" t="n">
-        <v>3</v>
+          <t>Other</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>Oryza sativa Japonica Group DNA, chromosome 9, cultivar: Nipponbare, complete sequence</t>
+        </is>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>Other</t>
+          <t>['hydroxycinnamoylputrescine']</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
         <is>
-          <t>Oryza sativa Japonica Group DNA, chromosome 9, cultivar: Nipponbare, complete sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L41" t="inlineStr">
         <is>
-          <t>hydroxycinnamoylputrescine</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M41" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.1</t>
+          <t>['Heterologous expression', 'Knock-out studies']</t>
         </is>
       </c>
       <c r="N41" t="inlineStr">
         <is>
           <t>['doi:10.1016/j.scib.2021.06.014']</t>
+        </is>
+      </c>
+      <c r="O41" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -3071,56 +3200,57 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>GPC_000011789.1</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
           <t>Hordeum vulgare subsp. vulgare</t>
         </is>
       </c>
+      <c r="E42" t="n">
+        <v>17320185</v>
+      </c>
       <c r="F42" t="n">
-        <v>17320184</v>
+        <v>17862889</v>
       </c>
       <c r="G42" t="n">
-        <v>17862889</v>
+        <v>4</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I42" t="n">
-        <v>5</v>
+          <t>Saccharide</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>Hordeum vulgare subsp. vulgare chromosome 1H, MorexV3_pseudomolecules_assembly, whole genome shotgun sequence</t>
+        </is>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Saccharide</t>
+          <t>['α-hydroxynitrile', 'glucoside', 'β-hydroxynitrile', 'glucoside', 'γ-hydroxynitrile', 'glucoside']</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
         <is>
-          <t>Hordeum vulgare subsp. vulgare chromosome 1H, MorexV3_pseudomolecules_assembly, whole genome shotgun sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L42" t="inlineStr">
         <is>
-          <t>α-hydroxynitrile</t>
-        </is>
-      </c>
-      <c r="M42" t="inlineStr">
-        <is>
-          <t>mibig_gbk_3.1</t>
-        </is>
-      </c>
+          <t>Unknown</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr"/>
       <c r="N42" t="inlineStr">
         <is>
           <t>['pubmed:27337134', 'doi:10.1111/tpj.13247']</t>
+        </is>
+      </c>
+      <c r="O42" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -3135,56 +3265,61 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>GPS_003181711.1</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
           <t>Saccharide</t>
         </is>
       </c>
+      <c r="E43" t="n">
+        <v>1123005</v>
+      </c>
       <c r="F43" t="n">
-        <v>1123004</v>
+        <v>1460949</v>
       </c>
       <c r="G43" t="n">
-        <v>1460949</v>
+        <v>22</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I43" t="n">
-        <v>22</v>
+          <t>Alkaloid</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>Solanum tuberosum cultivar DM 1-3 516 R44 unplaced genomic scaffold, SolTub_3.0 scf00140, whole genome shotgun sequence</t>
+        </is>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Alkaloid</t>
+          <t>['α-chaconine', 'α-solanine']</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
         <is>
-          <t>Solanum tuberosum cultivar DM 1-3 516 R44 unplaced genomic scaffold, SolTub_3.0 scf00140, whole genome shotgun sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L43" t="inlineStr">
         <is>
-          <t>α-chaconine,</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.1</t>
+          <t>['Heterologous expression', 'Gene expression correlated with compound production']</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
         <is>
           <t>['pubmed:23788733', 'doi:10.1126/science.1240230']</t>
+        </is>
+      </c>
+      <c r="O43" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -3199,56 +3334,61 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>GPS_020388126.1</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E44" t="inlineStr">
-        <is>
           <t>Jatropha curcas</t>
         </is>
       </c>
+      <c r="E44" t="n">
+        <v>7857</v>
+      </c>
       <c r="F44" t="n">
-        <v>7856</v>
+        <v>18675</v>
       </c>
       <c r="G44" t="n">
-        <v>18675</v>
+        <v>2</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I44" t="n">
-        <v>2</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>Jatropha curcas isolate ELGS0001-1231 unplaced genomic scaffold, RJC1_Hi-C scaffold_928, whole genome shotgun sequence</t>
+        </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['casbene']</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Jatropha curcas isolate ELGS0001-1231 unplaced genomic scaffold, RJC1_Hi-C scaffold_928, whole genome shotgun sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
         <is>
-          <t>casbene</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M44" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.1</t>
+          <t>['Heterologous expression']</t>
         </is>
       </c>
       <c r="N44" t="inlineStr">
         <is>
           <t>['pubmed:25172144', 'doi:10.1105/tpc.114.129668']</t>
+        </is>
+      </c>
+      <c r="O44" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>
@@ -3263,56 +3403,61 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>None</t>
+          <t>GPS_020388193.1</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="E45" t="inlineStr">
-        <is>
           <t>Jatropha curcas</t>
         </is>
       </c>
+      <c r="E45" t="n">
+        <v>848629</v>
+      </c>
       <c r="F45" t="n">
-        <v>848628</v>
+        <v>912207</v>
       </c>
       <c r="G45" t="n">
-        <v>912207</v>
+        <v>4</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="I45" t="n">
-        <v>6</v>
+          <t>Terpene</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>Jatropha curcas isolate ELGS0001-1231 unplaced genomic scaffold, RJC1_Hi-C scaffold_989, whole genome shotgun sequence</t>
+        </is>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>Terpene</t>
+          <t>['casbene']</t>
         </is>
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Jatropha curcas isolate ELGS0001-1231 unplaced genomic scaffold, RJC1_Hi-C scaffold_989, whole genome shotgun sequence</t>
+          <t>mibig_gbk_3.1</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
         <is>
-          <t>casbene</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="M45" t="inlineStr">
         <is>
-          <t>mibig_gbk_3.1</t>
+          <t>['Heterologous expression']</t>
         </is>
       </c>
       <c r="N45" t="inlineStr">
         <is>
           <t>['pubmed:25172144', 'doi:10.1105/tpc.114.129668']</t>
+        </is>
+      </c>
+      <c r="O45" t="inlineStr">
+        <is>
+          <t>[]</t>
         </is>
       </c>
     </row>

</xml_diff>